<commit_message>
Added additional recovery photos
</commit_message>
<xml_diff>
--- a/MISSION_DATA/A13_photos.xlsx
+++ b/MISSION_DATA/A13_photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apollo_13\MISSION_DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9676738E-99C2-4D3A-8CFD-5883179F09FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F2B575-BA5D-45D1-83E9-7FD0F1E132B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14700" yWindow="3885" windowWidth="31155" windowHeight="24675" xr2:uid="{E7285D04-3DFB-428F-BD58-901528569A82}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="1382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="1405">
   <si>
     <t>LM &amp; S-IVB during Transposition and Docking</t>
   </si>
@@ -4213,6 +4213,75 @@
   </si>
   <si>
     <t>Earth, Atlantic Ocean</t>
+  </si>
+  <si>
+    <t>S70-35562</t>
+  </si>
+  <si>
+    <t>146:12:38</t>
+  </si>
+  <si>
+    <t>S70-35562.jpg</t>
+  </si>
+  <si>
+    <t>Presidential Medal of Freedom article bestowed upon all of Mission Control.</t>
+  </si>
+  <si>
+    <t>S70-35603</t>
+  </si>
+  <si>
+    <t>S70-35603.jpg</t>
+  </si>
+  <si>
+    <t>143:42:45</t>
+  </si>
+  <si>
+    <t>Recovery prayer</t>
+  </si>
+  <si>
+    <t>S70-35629.jpg</t>
+  </si>
+  <si>
+    <t>S70-35629</t>
+  </si>
+  <si>
+    <t>143:43:32</t>
+  </si>
+  <si>
+    <t>S70-35652.jpg</t>
+  </si>
+  <si>
+    <t>S70-35652</t>
+  </si>
+  <si>
+    <t>On the mains</t>
+  </si>
+  <si>
+    <t>142:50:04</t>
+  </si>
+  <si>
+    <t>Splashdown</t>
+  </si>
+  <si>
+    <t>Thumbs up from Gerry Griffin</t>
+  </si>
+  <si>
+    <t>S70-35144.jpg</t>
+  </si>
+  <si>
+    <t>S70-35144</t>
+  </si>
+  <si>
+    <t>143:39:43</t>
+  </si>
+  <si>
+    <t>KSC-70PC-121.jpg</t>
+  </si>
+  <si>
+    <t>KSC-70PC-121</t>
+  </si>
+  <si>
+    <t>142:54:46</t>
   </si>
 </sst>
 </file>
@@ -4684,10 +4753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA25AE87-EBB6-4592-B83F-0D7E34AA70ED}">
-  <dimension ref="A1:H653"/>
+  <dimension ref="A1:H659"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A531" workbookViewId="0">
-      <selection activeCell="D570" sqref="D570"/>
+    <sheetView tabSelected="1" topLeftCell="A553" workbookViewId="0">
+      <selection activeCell="D580" sqref="D580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12374,28 +12443,28 @@
     </row>
     <row r="576" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A576" s="13" t="s">
-        <v>1212</v>
+        <v>1404</v>
       </c>
       <c r="B576" s="11" t="s">
-        <v>1083</v>
-      </c>
-      <c r="C576" s="11" t="s">
-        <v>1082</v>
-      </c>
-      <c r="D576" s="11"/>
+        <v>1403</v>
+      </c>
+      <c r="C576" s="11"/>
+      <c r="D576" s="11" t="s">
+        <v>1402</v>
+      </c>
       <c r="E576" s="11" t="s">
-        <v>1087</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="577" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A577" s="13" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B577" s="11" t="s">
-        <v>1069</v>
+        <v>1083</v>
       </c>
       <c r="C577" s="11" t="s">
-        <v>1058</v>
+        <v>1082</v>
       </c>
       <c r="D577" s="11"/>
       <c r="E577" s="11" t="s">
@@ -12404,283 +12473,283 @@
     </row>
     <row r="578" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A578" s="13" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B578" s="11" t="s">
-        <v>1104</v>
+        <v>1069</v>
       </c>
       <c r="C578" s="11" t="s">
-        <v>1103</v>
+        <v>1058</v>
       </c>
       <c r="D578" s="11"/>
       <c r="E578" s="11" t="s">
-        <v>1105</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="579" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A579" s="13" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B579" s="11" t="s">
-        <v>1073</v>
+        <v>1104</v>
       </c>
       <c r="C579" s="11" t="s">
-        <v>1081</v>
+        <v>1103</v>
       </c>
       <c r="D579" s="11"/>
       <c r="E579" s="11" t="s">
-        <v>1087</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A580" s="13" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B580" s="11" t="s">
-        <v>1101</v>
+        <v>1073</v>
       </c>
       <c r="C580" s="11" t="s">
-        <v>1100</v>
+        <v>1081</v>
       </c>
       <c r="D580" s="11"/>
       <c r="E580" s="11" t="s">
-        <v>1102</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A581" s="13" t="s">
-        <v>1275</v>
+        <v>1216</v>
       </c>
       <c r="B581" s="11" t="s">
-        <v>1229</v>
+        <v>1101</v>
       </c>
       <c r="C581" s="11" t="s">
-        <v>1228</v>
+        <v>1100</v>
       </c>
       <c r="D581" s="11"/>
       <c r="E581" s="11" t="s">
-        <v>1230</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A582" s="13" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="B582" s="11" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="C582" s="11" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="D582" s="11"/>
       <c r="E582" s="11" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="583" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A583" s="13" t="s">
-        <v>1286</v>
+        <v>1277</v>
       </c>
       <c r="B583" s="11" t="s">
-        <v>1265</v>
+        <v>1232</v>
       </c>
       <c r="C583" s="11" t="s">
-        <v>1264</v>
+        <v>1231</v>
       </c>
       <c r="D583" s="11"/>
       <c r="E583" s="11" t="s">
-        <v>1263</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A584" s="13" t="s">
-        <v>1051</v>
+        <v>1286</v>
       </c>
       <c r="B584" s="11" t="s">
-        <v>1261</v>
+        <v>1265</v>
       </c>
       <c r="C584" s="11" t="s">
-        <v>1260</v>
+        <v>1264</v>
       </c>
       <c r="D584" s="11"/>
       <c r="E584" s="11" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A585" s="13" t="s">
-        <v>1287</v>
+        <v>1051</v>
       </c>
       <c r="B585" s="11" t="s">
-        <v>1266</v>
+        <v>1261</v>
       </c>
       <c r="C585" s="11" t="s">
-        <v>1267</v>
+        <v>1260</v>
       </c>
       <c r="D585" s="11"/>
       <c r="E585" s="11" t="s">
-        <v>1268</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="586" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A586" s="13" t="s">
-        <v>1280</v>
+        <v>1287</v>
       </c>
       <c r="B586" s="11" t="s">
-        <v>1245</v>
+        <v>1266</v>
       </c>
       <c r="C586" s="11" t="s">
-        <v>1244</v>
+        <v>1267</v>
       </c>
       <c r="D586" s="11"/>
       <c r="E586" s="11" t="s">
-        <v>1243</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="587" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A587" s="13" t="s">
-        <v>1291</v>
+        <v>1280</v>
       </c>
       <c r="B587" s="11" t="s">
-        <v>1074</v>
-      </c>
-      <c r="C587" s="11"/>
-      <c r="D587" s="11" t="s">
-        <v>1290</v>
-      </c>
+        <v>1245</v>
+      </c>
+      <c r="C587" s="11" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D587" s="11"/>
       <c r="E587" s="11" t="s">
-        <v>1086</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A588" s="13" t="s">
-        <v>1288</v>
+        <v>1291</v>
       </c>
       <c r="B588" s="11" t="s">
-        <v>1270</v>
-      </c>
-      <c r="C588" s="11" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D588" s="11"/>
+        <v>1074</v>
+      </c>
+      <c r="C588" s="11"/>
+      <c r="D588" s="11" t="s">
+        <v>1290</v>
+      </c>
       <c r="E588" s="11" t="s">
-        <v>1271</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A589" s="13" t="s">
-        <v>1285</v>
+        <v>1288</v>
       </c>
       <c r="B589" s="11" t="s">
-        <v>1258</v>
+        <v>1270</v>
       </c>
       <c r="C589" s="11" t="s">
-        <v>1257</v>
+        <v>1269</v>
       </c>
       <c r="D589" s="11"/>
       <c r="E589" s="11" t="s">
-        <v>1259</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A590" s="13" t="s">
-        <v>1281</v>
+        <v>1285</v>
       </c>
       <c r="B590" s="11" t="s">
-        <v>1246</v>
+        <v>1258</v>
       </c>
       <c r="C590" s="11" t="s">
-        <v>1247</v>
+        <v>1257</v>
       </c>
       <c r="D590" s="11"/>
       <c r="E590" s="11" t="s">
-        <v>1248</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="591" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A591" s="13" t="s">
-        <v>1051</v>
+        <v>1281</v>
       </c>
       <c r="B591" s="11" t="s">
-        <v>1273</v>
+        <v>1246</v>
       </c>
       <c r="C591" s="11" t="s">
-        <v>1272</v>
+        <v>1247</v>
       </c>
       <c r="D591" s="11"/>
       <c r="E591" s="11" t="s">
-        <v>1274</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="592" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A592" s="13" t="s">
-        <v>1282</v>
+        <v>1051</v>
       </c>
       <c r="B592" s="11" t="s">
-        <v>1249</v>
+        <v>1273</v>
       </c>
       <c r="C592" s="11" t="s">
-        <v>1250</v>
+        <v>1272</v>
       </c>
       <c r="D592" s="11"/>
       <c r="E592" s="11" t="s">
-        <v>1248</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="593" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A593" s="13" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B593" s="11" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
       <c r="C593" s="11" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="D593" s="11"/>
       <c r="E593" s="11" t="s">
-        <v>1253</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="594" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A594" s="13" t="s">
-        <v>1217</v>
+        <v>1283</v>
       </c>
       <c r="B594" s="11" t="s">
-        <v>1070</v>
+        <v>1252</v>
       </c>
       <c r="C594" s="11" t="s">
-        <v>1059</v>
+        <v>1251</v>
       </c>
       <c r="D594" s="11"/>
       <c r="E594" s="11" t="s">
-        <v>1115</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="595" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A595" s="13" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B595" s="11" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="C595" s="11" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D595" s="11"/>
       <c r="E595" s="11" t="s">
-        <v>1087</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A596" s="13" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B596" s="11" t="s">
-        <v>1079</v>
+        <v>1071</v>
       </c>
       <c r="C596" s="11" t="s">
-        <v>1080</v>
+        <v>1060</v>
       </c>
       <c r="D596" s="11"/>
       <c r="E596" s="11" t="s">
@@ -12689,13 +12758,13 @@
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A597" s="13" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B597" s="11" t="s">
-        <v>1072</v>
+        <v>1079</v>
       </c>
       <c r="C597" s="11" t="s">
-        <v>1061</v>
+        <v>1080</v>
       </c>
       <c r="D597" s="11"/>
       <c r="E597" s="11" t="s">
@@ -12704,139 +12773,211 @@
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A598" s="13" t="s">
-        <v>1278</v>
+        <v>1220</v>
       </c>
       <c r="B598" s="11" t="s">
-        <v>1235</v>
+        <v>1072</v>
       </c>
       <c r="C598" s="11" t="s">
-        <v>1234</v>
+        <v>1061</v>
       </c>
       <c r="D598" s="11"/>
       <c r="E598" s="11" t="s">
-        <v>1236</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A599" s="13" t="s">
-        <v>1279</v>
+        <v>1401</v>
       </c>
       <c r="B599" s="11" t="s">
-        <v>1241</v>
-      </c>
-      <c r="C599" s="11" t="s">
-        <v>1240</v>
-      </c>
-      <c r="D599" s="11"/>
+        <v>1400</v>
+      </c>
+      <c r="C599" s="11"/>
+      <c r="D599" s="11" t="s">
+        <v>1399</v>
+      </c>
       <c r="E599" s="11" t="s">
-        <v>1242</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A600" s="13" t="s">
-        <v>1276</v>
+        <v>1278</v>
       </c>
       <c r="B600" s="11" t="s">
-        <v>1075</v>
+        <v>1235</v>
       </c>
       <c r="C600" s="11" t="s">
-        <v>1225</v>
+        <v>1234</v>
       </c>
       <c r="D600" s="11"/>
       <c r="E600" s="11" t="s">
-        <v>1086</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A601" s="13" t="s">
-        <v>1284</v>
+        <v>1383</v>
       </c>
       <c r="B601" s="11" t="s">
-        <v>1254</v>
-      </c>
-      <c r="C601" s="11" t="s">
-        <v>1256</v>
-      </c>
-      <c r="D601" s="11"/>
+        <v>1382</v>
+      </c>
+      <c r="C601" s="1"/>
+      <c r="D601" s="11" t="s">
+        <v>1384</v>
+      </c>
       <c r="E601" s="11" t="s">
-        <v>1255</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A602" s="13" t="s">
-        <v>1297</v>
+        <v>1388</v>
       </c>
       <c r="B602" s="11" t="s">
-        <v>1076</v>
-      </c>
-      <c r="C602" s="11"/>
+        <v>1386</v>
+      </c>
+      <c r="C602" s="1"/>
       <c r="D602" s="11" t="s">
-        <v>1294</v>
+        <v>1387</v>
       </c>
       <c r="E602" s="11" t="s">
-        <v>1086</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A603" s="13" t="s">
-        <v>1298</v>
+        <v>1279</v>
       </c>
       <c r="B603" s="11" t="s">
-        <v>1077</v>
-      </c>
-      <c r="C603" s="11"/>
-      <c r="D603" s="11" t="s">
-        <v>1295</v>
-      </c>
+        <v>1241</v>
+      </c>
+      <c r="C603" s="11" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D603" s="11"/>
       <c r="E603" s="11" t="s">
-        <v>1086</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="604" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A604" s="13" t="s">
-        <v>1299</v>
+        <v>1392</v>
       </c>
       <c r="B604" s="11" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C604" s="11"/>
+        <v>1391</v>
+      </c>
+      <c r="C604" s="1"/>
       <c r="D604" s="11" t="s">
-        <v>1296</v>
-      </c>
-      <c r="E604" s="11" t="s">
-        <v>1086</v>
-      </c>
+        <v>1390</v>
+      </c>
+      <c r="E604" s="11"/>
     </row>
     <row r="605" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A605" s="13" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B605" s="11" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C605" s="11" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D605" s="11"/>
+      <c r="E605" s="11" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="606" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A606" s="13" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B606" s="11" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C606" s="11" t="s">
+        <v>1256</v>
+      </c>
+      <c r="D606" s="11"/>
+      <c r="E606" s="11" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="607" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A607" s="13" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B607" s="11" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C607" s="11"/>
+      <c r="D607" s="11" t="s">
+        <v>1294</v>
+      </c>
+      <c r="E607" s="11" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="608" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A608" s="13" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B608" s="11" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C608" s="11"/>
+      <c r="D608" s="11" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E608" s="11" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="609" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A609" s="13" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B609" s="11" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C609" s="11"/>
+      <c r="D609" s="11" t="s">
+        <v>1296</v>
+      </c>
+      <c r="E609" s="11" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="610" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A610" s="13" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B610" s="11" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C610" s="11"/>
+      <c r="D610" s="11" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E610" s="11" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="611" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A611" s="13" t="s">
         <v>1293</v>
       </c>
-      <c r="B605" s="11" t="s">
+      <c r="B611" s="11" t="s">
         <v>1292</v>
       </c>
-      <c r="C605" s="11"/>
-      <c r="D605" s="11" t="s">
+      <c r="C611" s="11"/>
+      <c r="D611" s="11" t="s">
         <v>1292</v>
       </c>
-      <c r="E605" s="11"/>
-    </row>
-    <row r="643" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A643" s="14"/>
-    </row>
-    <row r="644" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A644" s="14"/>
-    </row>
-    <row r="645" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A645" s="14"/>
-    </row>
-    <row r="646" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A646" s="14"/>
-    </row>
-    <row r="647" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A647" s="14"/>
-    </row>
-    <row r="648" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A648" s="14"/>
+      <c r="E611" s="11" t="s">
+        <v>1397</v>
+      </c>
     </row>
     <row r="649" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A649" s="14"/>
@@ -12853,9 +12994,27 @@
     <row r="653" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A653" s="14"/>
     </row>
+    <row r="654" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A654" s="14"/>
+    </row>
+    <row r="655" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A655" s="14"/>
+    </row>
+    <row r="656" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A656" s="14"/>
+    </row>
+    <row r="657" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A657" s="14"/>
+    </row>
+    <row r="658" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A658" s="14"/>
+    </row>
+    <row r="659" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A659" s="14"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E607">
-    <sortCondition ref="B2:B607"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E613">
+    <sortCondition ref="B2:B613"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed flight photo display of photos with letters at the end of the filename
</commit_message>
<xml_diff>
--- a/MISSION_DATA/A13_photos.xlsx
+++ b/MISSION_DATA/A13_photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apollo_13\MISSION_DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F2B575-BA5D-45D1-83E9-7FD0F1E132B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F53C6F-F446-4BA4-A9ED-AFBABFFE1C53}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14700" yWindow="3885" windowWidth="31155" windowHeight="24675" xr2:uid="{E7285D04-3DFB-428F-BD58-901528569A82}"/>
   </bookViews>
@@ -4755,8 +4755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA25AE87-EBB6-4592-B83F-0D7E34AA70ED}">
   <dimension ref="A1:H659"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A553" workbookViewId="0">
-      <selection activeCell="D580" sqref="D580"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="A185" sqref="A185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
New photo timing from Robin Added some footage at very end
</commit_message>
<xml_diff>
--- a/MISSION_DATA/A13_photos.xlsx
+++ b/MISSION_DATA/A13_photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apollo_13\MISSION_DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C37D19C-BFB8-48D1-A94E-4964BE04344C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD654039-8405-4897-8750-7E8F06434CC0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14700" yWindow="3885" windowWidth="31155" windowHeight="24675" xr2:uid="{E7285D04-3DFB-428F-BD58-901528569A82}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="1408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="1409">
   <si>
     <t>LM &amp; S-IVB during Transposition and Docking</t>
   </si>
@@ -4291,6 +4291,9 @@
   </si>
   <si>
     <t>077:50:40</t>
+  </si>
+  <si>
+    <t>077:49:23</t>
   </si>
 </sst>
 </file>
@@ -7281,7 +7284,7 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="24" t="s">
-        <v>1312</v>
+        <v>1408</v>
       </c>
       <c r="B186" s="25" t="s">
         <v>695</v>

</xml_diff>

<commit_message>
BROKEN: modal broken somehow. Committing to troubleshoot
</commit_message>
<xml_diff>
--- a/MISSION_DATA/A13_photos.xlsx
+++ b/MISSION_DATA/A13_photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apollo_13\MISSION_DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD654039-8405-4897-8750-7E8F06434CC0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8917AB2A-3DCC-4C79-AEA7-4D8E5231558C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14700" yWindow="3885" windowWidth="31155" windowHeight="24675" xr2:uid="{E7285D04-3DFB-428F-BD58-901528569A82}"/>
   </bookViews>
@@ -3897,9 +3897,6 @@
     <t>143:43:29</t>
   </si>
   <si>
-    <t>143:57:03</t>
-  </si>
-  <si>
     <t>143:52:59</t>
   </si>
   <si>
@@ -4294,6 +4291,9 @@
   </si>
   <si>
     <t>077:49:23</t>
+  </si>
+  <si>
+    <t>143:57:34</t>
   </si>
 </sst>
 </file>
@@ -4776,8 +4776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA25AE87-EBB6-4592-B83F-0D7E34AA70ED}">
   <dimension ref="A1:H659"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B568"/>
+    <sheetView tabSelected="1" topLeftCell="A554" workbookViewId="0">
+      <selection activeCell="A587" sqref="A587"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4801,7 +4801,7 @@
         <v>1051</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>1048</v>
@@ -5220,7 +5220,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="B33" s="25" t="s">
         <v>1009</v>
@@ -5233,7 +5233,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="B34" s="25" t="s">
         <v>1010</v>
@@ -5254,7 +5254,7 @@
       <c r="C35" s="15"/>
       <c r="D35" s="16"/>
       <c r="E35" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -5267,7 +5267,7 @@
       <c r="C36" s="15"/>
       <c r="D36" s="16"/>
       <c r="E36" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -5280,7 +5280,7 @@
       <c r="C37" s="15"/>
       <c r="D37" s="16"/>
       <c r="E37" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -5293,7 +5293,7 @@
       <c r="C38" s="15"/>
       <c r="D38" s="16"/>
       <c r="E38" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -5306,7 +5306,7 @@
       <c r="C39" s="15"/>
       <c r="D39" s="16"/>
       <c r="E39" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -5319,7 +5319,7 @@
       <c r="C40" s="15"/>
       <c r="D40" s="16"/>
       <c r="E40" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -5332,7 +5332,7 @@
       <c r="C41" s="15"/>
       <c r="D41" s="16"/>
       <c r="E41" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -5345,7 +5345,7 @@
       <c r="C42" s="15"/>
       <c r="D42" s="16"/>
       <c r="E42" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -5358,7 +5358,7 @@
       <c r="C43" s="15"/>
       <c r="D43" s="16"/>
       <c r="E43" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -5371,7 +5371,7 @@
       <c r="C44" s="15"/>
       <c r="D44" s="16"/>
       <c r="E44" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -5384,7 +5384,7 @@
       <c r="C45" s="15"/>
       <c r="D45" s="16"/>
       <c r="E45" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -5397,7 +5397,7 @@
       <c r="C46" s="15"/>
       <c r="D46" s="16"/>
       <c r="E46" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -5410,7 +5410,7 @@
       <c r="C47" s="15"/>
       <c r="D47" s="16"/>
       <c r="E47" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -5423,7 +5423,7 @@
       <c r="C48" s="15"/>
       <c r="D48" s="16"/>
       <c r="E48" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -5436,7 +5436,7 @@
       <c r="C49" s="15"/>
       <c r="D49" s="16"/>
       <c r="E49" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -5449,7 +5449,7 @@
       <c r="C50" s="15"/>
       <c r="D50" s="16"/>
       <c r="E50" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -5462,7 +5462,7 @@
       <c r="C51" s="15"/>
       <c r="D51" s="16"/>
       <c r="E51" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="52" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
@@ -5475,7 +5475,7 @@
       <c r="C52" s="15"/>
       <c r="D52" s="16"/>
       <c r="E52" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="F52" s="1"/>
     </row>
@@ -5489,13 +5489,13 @@
       <c r="C53" s="15"/>
       <c r="D53" s="16"/>
       <c r="E53" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="B54" s="25" t="s">
         <v>1008</v>
@@ -5503,7 +5503,7 @@
       <c r="C54" s="15"/>
       <c r="D54" s="16"/>
       <c r="E54" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="F54" s="1"/>
     </row>
@@ -5517,7 +5517,7 @@
       <c r="C55" s="15"/>
       <c r="D55" s="16"/>
       <c r="E55" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="F55" s="1"/>
     </row>
@@ -5531,7 +5531,7 @@
       <c r="C56" s="15"/>
       <c r="D56" s="16"/>
       <c r="E56" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -5544,7 +5544,7 @@
       <c r="C57" s="15"/>
       <c r="D57" s="16"/>
       <c r="E57" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -5557,7 +5557,7 @@
       <c r="C58" s="15"/>
       <c r="D58" s="16"/>
       <c r="E58" s="18" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -5570,7 +5570,7 @@
       <c r="C59" s="15"/>
       <c r="D59" s="16"/>
       <c r="E59" s="18" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -5583,7 +5583,7 @@
       <c r="C60" s="15"/>
       <c r="D60" s="16"/>
       <c r="E60" s="18" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -5596,7 +5596,7 @@
       <c r="C61" s="15"/>
       <c r="D61" s="16"/>
       <c r="E61" s="18" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -5609,7 +5609,7 @@
       <c r="C62" s="15"/>
       <c r="D62" s="16"/>
       <c r="E62" s="18" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -5622,7 +5622,7 @@
       <c r="C63" s="15"/>
       <c r="D63" s="16"/>
       <c r="E63" s="18" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -5635,7 +5635,7 @@
       <c r="C64" s="15"/>
       <c r="D64" s="16"/>
       <c r="E64" s="18" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -5648,7 +5648,7 @@
       <c r="C65" s="15"/>
       <c r="D65" s="16"/>
       <c r="E65" s="18" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -5661,7 +5661,7 @@
       <c r="C66" s="15"/>
       <c r="D66" s="16"/>
       <c r="E66" s="18" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -5674,7 +5674,7 @@
       <c r="C67" s="15"/>
       <c r="D67" s="16"/>
       <c r="E67" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -5687,7 +5687,7 @@
       <c r="C68" s="15"/>
       <c r="D68" s="16"/>
       <c r="E68" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -5700,7 +5700,7 @@
       <c r="C69" s="15"/>
       <c r="D69" s="16"/>
       <c r="E69" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="70" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
@@ -5713,7 +5713,7 @@
       <c r="C70" s="15"/>
       <c r="D70" s="16"/>
       <c r="E70" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F70" s="1"/>
     </row>
@@ -5727,7 +5727,7 @@
       <c r="C71" s="15"/>
       <c r="D71" s="16"/>
       <c r="E71" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F71" s="1"/>
     </row>
@@ -5741,7 +5741,7 @@
       <c r="C72" s="15"/>
       <c r="D72" s="16"/>
       <c r="E72" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F72" s="1"/>
     </row>
@@ -5755,7 +5755,7 @@
       <c r="C73" s="15"/>
       <c r="D73" s="16"/>
       <c r="E73" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F73" s="1"/>
     </row>
@@ -5769,7 +5769,7 @@
       <c r="C74" s="15"/>
       <c r="D74" s="16"/>
       <c r="E74" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F74" s="1"/>
     </row>
@@ -5783,7 +5783,7 @@
       <c r="C75" s="15"/>
       <c r="D75" s="16"/>
       <c r="E75" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F75" s="1"/>
     </row>
@@ -5797,7 +5797,7 @@
       <c r="C76" s="15"/>
       <c r="D76" s="16"/>
       <c r="E76" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F76" s="1"/>
     </row>
@@ -5811,7 +5811,7 @@
       <c r="C77" s="15"/>
       <c r="D77" s="16"/>
       <c r="E77" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F77" s="1"/>
     </row>
@@ -5825,7 +5825,7 @@
       <c r="C78" s="15"/>
       <c r="D78" s="16"/>
       <c r="E78" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F78" s="1"/>
     </row>
@@ -5839,7 +5839,7 @@
       <c r="C79" s="15"/>
       <c r="D79" s="16"/>
       <c r="E79" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F79" s="1"/>
     </row>
@@ -5853,7 +5853,7 @@
       <c r="C80" s="15"/>
       <c r="D80" s="16"/>
       <c r="E80" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F80" s="1"/>
     </row>
@@ -5867,7 +5867,7 @@
       <c r="C81" s="15"/>
       <c r="D81" s="16"/>
       <c r="E81" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F81" s="1"/>
     </row>
@@ -5881,7 +5881,7 @@
       <c r="C82" s="15"/>
       <c r="D82" s="16"/>
       <c r="E82" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F82" s="1"/>
     </row>
@@ -5895,7 +5895,7 @@
       <c r="C83" s="15"/>
       <c r="D83" s="16"/>
       <c r="E83" s="18" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="F83" s="1"/>
     </row>
@@ -5909,7 +5909,7 @@
       <c r="C84" s="15"/>
       <c r="D84" s="16"/>
       <c r="E84" s="18" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="F84" s="1"/>
     </row>
@@ -5923,13 +5923,13 @@
       <c r="C85" s="15"/>
       <c r="D85" s="16"/>
       <c r="E85" s="18" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="24" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="B86" s="25" t="s">
         <v>489</v>
@@ -6069,7 +6069,7 @@
     </row>
     <row r="96" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="24" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="B96" s="25" t="s">
         <v>499</v>
@@ -6083,7 +6083,7 @@
     </row>
     <row r="97" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="24" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="B97" s="25" t="s">
         <v>500</v>
@@ -6097,7 +6097,7 @@
     </row>
     <row r="98" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="24" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="B98" s="25" t="s">
         <v>501</v>
@@ -6119,7 +6119,7 @@
       <c r="C99" s="15"/>
       <c r="D99" s="16"/>
       <c r="E99" s="18" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="F99" s="1"/>
     </row>
@@ -6133,7 +6133,7 @@
       <c r="C100" s="15"/>
       <c r="D100" s="16"/>
       <c r="E100" s="20" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="F100" s="1"/>
     </row>
@@ -6147,7 +6147,7 @@
       <c r="C101" s="15"/>
       <c r="D101" s="16"/>
       <c r="E101" s="20" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="F101" s="1"/>
     </row>
@@ -6161,7 +6161,7 @@
       <c r="C102" s="15"/>
       <c r="D102" s="16"/>
       <c r="E102" s="20" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="F102" s="1"/>
     </row>
@@ -6175,7 +6175,7 @@
       <c r="C103" s="15"/>
       <c r="D103" s="16"/>
       <c r="E103" s="20" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="F103" s="1"/>
     </row>
@@ -6189,7 +6189,7 @@
       <c r="C104" s="15"/>
       <c r="D104" s="16"/>
       <c r="E104" s="20" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="105" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
@@ -6202,7 +6202,7 @@
       <c r="C105" s="15"/>
       <c r="D105" s="16"/>
       <c r="E105" s="20" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="F105" s="1"/>
     </row>
@@ -6216,7 +6216,7 @@
       <c r="C106" s="15"/>
       <c r="D106" s="16"/>
       <c r="E106" s="20" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="107" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
@@ -6229,7 +6229,7 @@
       <c r="C107" s="15"/>
       <c r="D107" s="16"/>
       <c r="E107" s="20" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="F107" s="1"/>
     </row>
@@ -6243,7 +6243,7 @@
       <c r="C108" s="15"/>
       <c r="D108" s="16"/>
       <c r="E108" s="20" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -6261,7 +6261,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="24" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="B110" s="25" t="s">
         <v>513</v>
@@ -6274,7 +6274,7 @@
     </row>
     <row r="111" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="24" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B111" s="25" t="s">
         <v>514</v>
@@ -6288,7 +6288,7 @@
     </row>
     <row r="112" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="24" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B112" s="25" t="s">
         <v>536</v>
@@ -7215,7 +7215,7 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="24" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B181" s="25" t="s">
         <v>668</v>
@@ -7254,7 +7254,7 @@
     </row>
     <row r="184" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="24" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="B184" s="25" t="s">
         <v>680</v>
@@ -7284,7 +7284,7 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="24" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="B186" s="25" t="s">
         <v>695</v>
@@ -7310,7 +7310,7 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="24" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="B188" s="25" t="s">
         <v>778</v>
@@ -7323,7 +7323,7 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="24" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="B189" s="25" t="s">
         <v>780</v>
@@ -7336,7 +7336,7 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="24" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="B190" s="25" t="s">
         <v>782</v>
@@ -7364,7 +7364,7 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="24" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="B192" s="25" t="s">
         <v>789</v>
@@ -7377,7 +7377,7 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="24" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="B193" s="25" t="s">
         <v>791</v>
@@ -7390,7 +7390,7 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="24" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="B194" s="25" t="s">
         <v>792</v>
@@ -7403,7 +7403,7 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="24" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="B195" s="25" t="s">
         <v>793</v>
@@ -7416,7 +7416,7 @@
     </row>
     <row r="196" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="24" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="B196" s="25" t="s">
         <v>794</v>
@@ -7431,7 +7431,7 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="24" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="B197" s="25" t="s">
         <v>795</v>
@@ -7444,7 +7444,7 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="24" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="B198" s="25" t="s">
         <v>796</v>
@@ -7457,7 +7457,7 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="24" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B199" s="25" t="s">
         <v>797</v>
@@ -7470,7 +7470,7 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="24" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="B200" s="25" t="s">
         <v>798</v>
@@ -7483,7 +7483,7 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="24" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="B201" s="25" t="s">
         <v>799</v>
@@ -7496,7 +7496,7 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="24" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="B202" s="25" t="s">
         <v>800</v>
@@ -7509,7 +7509,7 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="24" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="B203" s="25" t="s">
         <v>801</v>
@@ -7522,7 +7522,7 @@
     </row>
     <row r="204" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="24" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="B204" s="25" t="s">
         <v>802</v>
@@ -7537,7 +7537,7 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="24" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="B205" s="25" t="s">
         <v>803</v>
@@ -7550,7 +7550,7 @@
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="24" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="B206" s="25" t="s">
         <v>805</v>
@@ -7563,7 +7563,7 @@
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="24" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="B207" s="25" t="s">
         <v>808</v>
@@ -7576,7 +7576,7 @@
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="24" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B208" s="25" t="s">
         <v>809</v>
@@ -7589,7 +7589,7 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="24" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="B209" s="25" t="s">
         <v>813</v>
@@ -7602,7 +7602,7 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="24" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="B210" s="25" t="s">
         <v>814</v>
@@ -7615,7 +7615,7 @@
     </row>
     <row r="211" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="24" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B211" s="25" t="s">
         <v>815</v>
@@ -7630,7 +7630,7 @@
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="24" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B212" s="25" t="s">
         <v>816</v>
@@ -7643,7 +7643,7 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="24" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B213" s="25" t="s">
         <v>817</v>
@@ -7656,7 +7656,7 @@
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="24" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B214" s="25" t="s">
         <v>818</v>
@@ -7794,7 +7794,7 @@
       <c r="C224" s="15"/>
       <c r="D224" s="16"/>
       <c r="E224" s="18" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -7807,7 +7807,7 @@
       <c r="C225" s="15"/>
       <c r="D225" s="16"/>
       <c r="E225" s="18" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -7937,7 +7937,7 @@
       <c r="C235" s="15"/>
       <c r="D235" s="16"/>
       <c r="E235" s="21" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -7950,7 +7950,7 @@
       <c r="C236" s="15"/>
       <c r="D236" s="16"/>
       <c r="E236" s="21" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -7963,12 +7963,12 @@
       <c r="C237" s="15"/>
       <c r="D237" s="16"/>
       <c r="E237" s="21" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="24" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B238" s="25" t="s">
         <v>617</v>
@@ -8020,7 +8020,7 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="24" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B242" s="25" t="s">
         <v>621</v>
@@ -8067,7 +8067,7 @@
       <c r="C245" s="15"/>
       <c r="D245" s="16"/>
       <c r="E245" s="21" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -8080,7 +8080,7 @@
       <c r="C246" s="15"/>
       <c r="D246" s="16"/>
       <c r="E246" s="21" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -8280,7 +8280,7 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="24" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="B262" s="25" t="s">
         <v>653</v>
@@ -8566,7 +8566,7 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="24" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="B284" s="25" t="s">
         <v>681</v>
@@ -8592,7 +8592,7 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="24" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="B286" s="25" t="s">
         <v>683</v>
@@ -8605,7 +8605,7 @@
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="24" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="B287" s="25" t="s">
         <v>684</v>
@@ -8907,7 +8907,7 @@
     </row>
     <row r="309" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A309" s="24" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="B309" s="25" t="s">
         <v>708</v>
@@ -8922,7 +8922,7 @@
     </row>
     <row r="310" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A310" s="24" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="B310" s="25" t="s">
         <v>709</v>
@@ -8967,7 +8967,7 @@
     </row>
     <row r="313" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A313" s="24" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="B313" s="25" t="s">
         <v>712</v>
@@ -8982,7 +8982,7 @@
     </row>
     <row r="314" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A314" s="24" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="B314" s="25" t="s">
         <v>713</v>
@@ -9195,7 +9195,7 @@
     </row>
     <row r="329" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A329" s="25" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="B329" s="25" t="s">
         <v>728</v>
@@ -9225,7 +9225,7 @@
     </row>
     <row r="331" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A331" s="24" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="B331" s="25" t="s">
         <v>730</v>
@@ -9240,7 +9240,7 @@
     </row>
     <row r="332" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A332" s="24" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="B332" s="25" t="s">
         <v>731</v>
@@ -9255,7 +9255,7 @@
     </row>
     <row r="333" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A333" s="24" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B333" s="25" t="s">
         <v>732</v>
@@ -9270,7 +9270,7 @@
     </row>
     <row r="334" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A334" s="24" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="B334" s="25" t="s">
         <v>733</v>
@@ -9285,7 +9285,7 @@
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A335" s="24" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="B335" s="25" t="s">
         <v>734</v>
@@ -9298,7 +9298,7 @@
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A336" s="24" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="B336" s="25" t="s">
         <v>735</v>
@@ -9311,7 +9311,7 @@
     </row>
     <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337" s="24" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="B337" s="25" t="s">
         <v>736</v>
@@ -9324,7 +9324,7 @@
     </row>
     <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" s="24" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B338" s="25" t="s">
         <v>737</v>
@@ -9337,7 +9337,7 @@
     </row>
     <row r="339" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A339" s="24" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B339" s="25" t="s">
         <v>738</v>
@@ -9352,7 +9352,7 @@
     </row>
     <row r="340" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A340" s="24" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B340" s="25" t="s">
         <v>739</v>
@@ -9367,7 +9367,7 @@
     </row>
     <row r="341" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A341" s="23" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="B341" s="25" t="s">
         <v>740</v>
@@ -9382,7 +9382,7 @@
     </row>
     <row r="342" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A342" s="24" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="B342" s="25" t="s">
         <v>741</v>
@@ -9397,7 +9397,7 @@
     </row>
     <row r="343" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A343" s="23" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="B343" s="25" t="s">
         <v>742</v>
@@ -10004,7 +10004,7 @@
       <c r="C387" s="15"/>
       <c r="D387" s="16"/>
       <c r="E387" s="18" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="388" spans="1:6" x14ac:dyDescent="0.25">
@@ -10043,7 +10043,7 @@
       <c r="C390" s="15"/>
       <c r="D390" s="16"/>
       <c r="E390" s="18" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="391" spans="1:6" x14ac:dyDescent="0.25">
@@ -10056,7 +10056,7 @@
       <c r="C391" s="15"/>
       <c r="D391" s="16"/>
       <c r="E391" s="18" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="392" spans="1:6" x14ac:dyDescent="0.25">
@@ -10069,7 +10069,7 @@
       <c r="C392" s="15"/>
       <c r="D392" s="16"/>
       <c r="E392" s="18" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="393" spans="1:6" x14ac:dyDescent="0.25">
@@ -10082,7 +10082,7 @@
       <c r="C393" s="15"/>
       <c r="D393" s="16"/>
       <c r="E393" s="18" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="394" spans="1:6" x14ac:dyDescent="0.25">
@@ -10095,7 +10095,7 @@
       <c r="C394" s="15"/>
       <c r="D394" s="16"/>
       <c r="E394" s="18" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="395" spans="1:6" x14ac:dyDescent="0.25">
@@ -10108,7 +10108,7 @@
       <c r="C395" s="15"/>
       <c r="D395" s="16"/>
       <c r="E395" s="18" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="396" spans="1:6" x14ac:dyDescent="0.25">
@@ -10121,7 +10121,7 @@
       <c r="C396" s="15"/>
       <c r="D396" s="16"/>
       <c r="E396" s="18" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="397" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
@@ -10134,13 +10134,13 @@
       <c r="C397" s="15"/>
       <c r="D397" s="16"/>
       <c r="E397" s="18" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="F397" s="1"/>
     </row>
     <row r="398" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A398" s="24" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="B398" s="25" t="s">
         <v>850</v>
@@ -10154,7 +10154,7 @@
     </row>
     <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399" s="24" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="B399" s="25" t="s">
         <v>851</v>
@@ -10167,7 +10167,7 @@
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A400" s="24" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="B400" s="25" t="s">
         <v>852</v>
@@ -10180,7 +10180,7 @@
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A401" s="24" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="B401" s="25" t="s">
         <v>853</v>
@@ -10193,7 +10193,7 @@
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A402" s="25" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="B402" s="25" t="s">
         <v>515</v>
@@ -10232,7 +10232,7 @@
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A405" s="27" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="B405" s="25" t="s">
         <v>518</v>
@@ -10310,7 +10310,7 @@
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A411" s="25" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="B411" s="25" t="s">
         <v>524</v>
@@ -10427,7 +10427,7 @@
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A420" s="25" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="B420" s="25" t="s">
         <v>533</v>
@@ -10440,7 +10440,7 @@
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A421" s="25" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="B421" s="25" t="s">
         <v>534</v>
@@ -10453,7 +10453,7 @@
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A422" s="25" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="B422" s="25" t="s">
         <v>535</v>
@@ -10474,7 +10474,7 @@
       <c r="C423" s="15"/>
       <c r="D423" s="16"/>
       <c r="E423" s="18" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.25">
@@ -10487,7 +10487,7 @@
       <c r="C424" s="15"/>
       <c r="D424" s="16"/>
       <c r="E424" s="18" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
@@ -10500,7 +10500,7 @@
       <c r="C425" s="15"/>
       <c r="D425" s="16"/>
       <c r="E425" s="18" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
@@ -10513,7 +10513,7 @@
       <c r="C426" s="15"/>
       <c r="D426" s="16"/>
       <c r="E426" s="18" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.25">
@@ -10526,7 +10526,7 @@
       <c r="C427" s="15"/>
       <c r="D427" s="16"/>
       <c r="E427" s="18" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
@@ -10539,7 +10539,7 @@
       <c r="C428" s="15"/>
       <c r="D428" s="16"/>
       <c r="E428" s="18" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
@@ -10830,7 +10830,7 @@
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A451" s="25" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="B451" s="25" t="s">
         <v>843</v>
@@ -10843,7 +10843,7 @@
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A452" s="25" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="B452" s="25" t="s">
         <v>844</v>
@@ -12191,7 +12191,7 @@
       <c r="C555" s="15"/>
       <c r="D555" s="16"/>
       <c r="E555" s="18" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="556" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -12204,7 +12204,7 @@
       <c r="C556" s="15"/>
       <c r="D556" s="16"/>
       <c r="E556" s="18" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="557" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -12230,7 +12230,7 @@
       <c r="C558" s="15"/>
       <c r="D558" s="16"/>
       <c r="E558" s="18" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="559" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -12243,7 +12243,7 @@
       <c r="C559" s="15"/>
       <c r="D559" s="16"/>
       <c r="E559" s="18" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="560" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -12256,7 +12256,7 @@
       <c r="C560" s="15"/>
       <c r="D560" s="16"/>
       <c r="E560" s="18" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="561" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -12464,17 +12464,17 @@
     </row>
     <row r="576" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A576" s="13" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B576" s="11" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="C576" s="11"/>
       <c r="D576" s="11" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="E576" s="11" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="577" spans="1:5" x14ac:dyDescent="0.25">
@@ -12584,7 +12584,7 @@
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A584" s="13" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B584" s="11" t="s">
         <v>1261</v>
@@ -12614,7 +12614,7 @@
     </row>
     <row r="586" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A586" s="13" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B586" s="11" t="s">
         <v>1262</v>
@@ -12629,7 +12629,7 @@
     </row>
     <row r="587" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A587" s="13" t="s">
-        <v>1276</v>
+        <v>1408</v>
       </c>
       <c r="B587" s="11" t="s">
         <v>1241</v>
@@ -12644,14 +12644,14 @@
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A588" s="13" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B588" s="11" t="s">
         <v>1072</v>
       </c>
       <c r="C588" s="11"/>
       <c r="D588" s="11" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="E588" s="11" t="s">
         <v>1084</v>
@@ -12659,7 +12659,7 @@
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A589" s="13" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B589" s="11" t="s">
         <v>1266</v>
@@ -12674,7 +12674,7 @@
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A590" s="13" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="B590" s="11" t="s">
         <v>1254</v>
@@ -12689,7 +12689,7 @@
     </row>
     <row r="591" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A591" s="13" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="B591" s="11" t="s">
         <v>1242</v>
@@ -12719,7 +12719,7 @@
     </row>
     <row r="593" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A593" s="13" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="B593" s="11" t="s">
         <v>1245</v>
@@ -12734,7 +12734,7 @@
     </row>
     <row r="594" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A594" s="13" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="B594" s="11" t="s">
         <v>1248</v>
@@ -12809,17 +12809,17 @@
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A599" s="13" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="B599" s="11" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="C599" s="11"/>
       <c r="D599" s="11" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="E599" s="11" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
@@ -12839,32 +12839,32 @@
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A601" s="13" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B601" s="11" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="C601" s="1"/>
       <c r="D601" s="11" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E601" s="11" t="s">
         <v>1380</v>
-      </c>
-      <c r="E601" s="11" t="s">
-        <v>1381</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A602" s="13" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="B602" s="11" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="C602" s="1"/>
       <c r="D602" s="11" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="E602" s="11" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.25">
@@ -12884,14 +12884,14 @@
     </row>
     <row r="604" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A604" s="13" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="B604" s="11" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="C604" s="1"/>
       <c r="D604" s="11" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="E604" s="11"/>
     </row>
@@ -12912,7 +12912,7 @@
     </row>
     <row r="606" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A606" s="13" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="B606" s="11" t="s">
         <v>1250</v>
@@ -12927,14 +12927,14 @@
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A607" s="13" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="B607" s="11" t="s">
         <v>1074</v>
       </c>
       <c r="C607" s="11"/>
       <c r="D607" s="11" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="E607" s="11" t="s">
         <v>1084</v>
@@ -12942,14 +12942,14 @@
     </row>
     <row r="608" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A608" s="13" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="B608" s="11" t="s">
         <v>1075</v>
       </c>
       <c r="C608" s="11"/>
       <c r="D608" s="11" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="E608" s="11" t="s">
         <v>1084</v>
@@ -12957,14 +12957,14 @@
     </row>
     <row r="609" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A609" s="13" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="B609" s="11" t="s">
         <v>1076</v>
       </c>
       <c r="C609" s="11"/>
       <c r="D609" s="11" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="E609" s="11" t="s">
         <v>1084</v>
@@ -12972,32 +12972,32 @@
     </row>
     <row r="610" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A610" s="13" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="B610" s="11" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="C610" s="11"/>
       <c r="D610" s="11" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="E610" s="11" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="611" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A611" s="13" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B611" s="11" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="C611" s="11"/>
       <c r="D611" s="11" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="E611" s="11" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="649" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates after 708 delivery Premiere period during explosion retimed
</commit_message>
<xml_diff>
--- a/MISSION_DATA/A13_photos.xlsx
+++ b/MISSION_DATA/A13_photos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apollo_13\MISSION_DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9D87C4-D980-4EF2-A9A7-4BFE2E42A96A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E071D29-B9E5-4A53-A940-C81E9DE461E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10050" yWindow="2850" windowWidth="33000" windowHeight="29265" xr2:uid="{E7285D04-3DFB-428F-BD58-901528569A82}"/>
+    <workbookView xWindow="10500" yWindow="4260" windowWidth="28920" windowHeight="23985" xr2:uid="{E7285D04-3DFB-428F-BD58-901528569A82}"/>
   </bookViews>
   <sheets>
     <sheet name="A13_photos" sheetId="15" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4011" uniqueCount="1725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4015" uniqueCount="1766">
   <si>
     <t>LM &amp; S-IVB during Transposition and Docking</t>
   </si>
@@ -5243,6 +5243,129 @@
   </si>
   <si>
     <t>077:38:02</t>
+  </si>
+  <si>
+    <t>003:12:55</t>
+  </si>
+  <si>
+    <t>003:13:10</t>
+  </si>
+  <si>
+    <t>003:13:36</t>
+  </si>
+  <si>
+    <t>004:10:12</t>
+  </si>
+  <si>
+    <t>004:10:55</t>
+  </si>
+  <si>
+    <t>004:11:15</t>
+  </si>
+  <si>
+    <t>004:12:10</t>
+  </si>
+  <si>
+    <t>004:12:31</t>
+  </si>
+  <si>
+    <t>004:15:51</t>
+  </si>
+  <si>
+    <t>080:51:58</t>
+  </si>
+  <si>
+    <t>080:52:20</t>
+  </si>
+  <si>
+    <t>080:52:37</t>
+  </si>
+  <si>
+    <t>080:52:59</t>
+  </si>
+  <si>
+    <t>080:53:22</t>
+  </si>
+  <si>
+    <t>080:53:40</t>
+  </si>
+  <si>
+    <t>083:25:15</t>
+  </si>
+  <si>
+    <t>083:25:35</t>
+  </si>
+  <si>
+    <t>083:31:10</t>
+  </si>
+  <si>
+    <t>083:31:28</t>
+  </si>
+  <si>
+    <t>099:15:15</t>
+  </si>
+  <si>
+    <t>099:17:04</t>
+  </si>
+  <si>
+    <t>080:36:33</t>
+  </si>
+  <si>
+    <t>080:36:37</t>
+  </si>
+  <si>
+    <t>080:36:45</t>
+  </si>
+  <si>
+    <t>080:36:50</t>
+  </si>
+  <si>
+    <t>080:36:54</t>
+  </si>
+  <si>
+    <t>081:34:30</t>
+  </si>
+  <si>
+    <t>081:34:41</t>
+  </si>
+  <si>
+    <t>081:35:08</t>
+  </si>
+  <si>
+    <t>081:35:20</t>
+  </si>
+  <si>
+    <t>081:36:02</t>
+  </si>
+  <si>
+    <t>081:43:18</t>
+  </si>
+  <si>
+    <t>081:43:29</t>
+  </si>
+  <si>
+    <t>068:00:45</t>
+  </si>
+  <si>
+    <t>068:04:10</t>
+  </si>
+  <si>
+    <t>094:19:06</t>
+  </si>
+  <si>
+    <t>094:19:28</t>
+  </si>
+  <si>
+    <t>099:38:46</t>
+  </si>
+  <si>
+    <t>098:39:01</t>
+  </si>
+  <si>
+    <t>099:39:28</t>
+  </si>
+  <si>
+    <t>099:40:32</t>
   </si>
 </sst>
 </file>
@@ -5722,8 +5845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA25AE87-EBB6-4592-B83F-0D7E34AA70ED}">
   <dimension ref="A1:H704"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A566" workbookViewId="0">
-      <selection activeCell="B615" sqref="B615"/>
+    <sheetView tabSelected="1" topLeftCell="A646" workbookViewId="0">
+      <selection activeCell="D667" sqref="D667"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6101,7 +6224,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="31">
-        <v>5.7540393518518513</v>
+        <v>5.7540856481481484</v>
       </c>
       <c r="B28" t="s">
         <v>792</v>
@@ -6114,7 +6237,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="31">
-        <v>5.7540509259259265</v>
+        <v>5.7541203703703703</v>
       </c>
       <c r="B29" t="s">
         <v>793</v>
@@ -6127,7 +6250,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="31">
-        <v>5.7540624999999999</v>
+        <v>5.7541782407407416</v>
       </c>
       <c r="B30" t="s">
         <v>795</v>
@@ -6140,7 +6263,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="31">
-        <v>5.7540856481481484</v>
+        <v>5.7542013888888883</v>
       </c>
       <c r="B31" t="s">
         <v>1178</v>
@@ -6153,7 +6276,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="31">
-        <v>5.7540972222222218</v>
+        <v>5.7542129629629635</v>
       </c>
       <c r="B32" t="s">
         <v>797</v>
@@ -6166,7 +6289,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="31">
-        <v>5.754108796296296</v>
+        <v>5.7542245370370368</v>
       </c>
       <c r="B33" t="s">
         <v>799</v>
@@ -6179,7 +6302,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="31">
-        <v>5.7541203703703703</v>
+        <v>5.7542592592592596</v>
       </c>
       <c r="B34" t="s">
         <v>801</v>
@@ -6192,7 +6315,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="31">
-        <v>5.7541435185185188</v>
+        <v>5.7542824074074082</v>
       </c>
       <c r="B35" t="s">
         <v>802</v>
@@ -6335,7 +6458,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="31">
-        <v>5.6805092592592592</v>
+        <v>5.6791203703703701</v>
       </c>
       <c r="B46" t="s">
         <v>1161</v>
@@ -6348,7 +6471,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="31">
-        <v>5.6807291666666666</v>
+        <v>5.6793402777777784</v>
       </c>
       <c r="B47" t="s">
         <v>1155</v>
@@ -6361,7 +6484,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="31">
-        <v>5.6808796296296293</v>
+        <v>5.6794907407407402</v>
       </c>
       <c r="B48" t="s">
         <v>1156</v>
@@ -6374,7 +6497,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="31">
-        <v>5.6810416666666663</v>
+        <v>5.6796527777777781</v>
       </c>
       <c r="B49" t="s">
         <v>1157</v>
@@ -6387,7 +6510,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="31">
-        <v>5.6812268518518527</v>
+        <v>5.6798379629629627</v>
       </c>
       <c r="B50" t="s">
         <v>1158</v>
@@ -6400,7 +6523,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="31">
-        <v>5.6813888888888888</v>
+        <v>5.68</v>
       </c>
       <c r="B51" t="s">
         <v>1152</v>
@@ -6413,7 +6536,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="31">
-        <v>5.6815740740740743</v>
+        <v>5.6801851851851852</v>
       </c>
       <c r="B52" t="s">
         <v>1153</v>
@@ -6426,7 +6549,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="31">
-        <v>5.6817129629629628</v>
+        <v>5.6803240740740746</v>
       </c>
       <c r="B53" t="s">
         <v>1154</v>
@@ -6556,7 +6679,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="31">
-        <v>5.7537384259259268</v>
+        <v>5.7539583333333333</v>
       </c>
       <c r="B63" t="s">
         <v>1142</v>
@@ -6569,7 +6692,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="31">
-        <v>5.7537615740740735</v>
+        <v>5.7539814814814818</v>
       </c>
       <c r="B64" t="s">
         <v>1141</v>
@@ -6582,7 +6705,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="31">
-        <v>5.7538541666666667</v>
+        <v>5.7540393518518513</v>
       </c>
       <c r="B65" t="s">
         <v>1138</v>
@@ -6595,7 +6718,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="31">
-        <v>5.7538888888888886</v>
+        <v>5.7540624999999999</v>
       </c>
       <c r="B66" t="s">
         <v>1139</v>
@@ -6608,7 +6731,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="31">
-        <v>5.7539120370370371</v>
+        <v>5.754108796296296</v>
       </c>
       <c r="B67" t="s">
         <v>1140</v>
@@ -6621,7 +6744,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="31">
-        <v>5.7539351851851848</v>
+        <v>5.7541435185185188</v>
       </c>
       <c r="B68" t="s">
         <v>1135</v>
@@ -6634,7 +6757,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="31">
-        <v>5.7539583333333333</v>
+        <v>5.7541550925925931</v>
       </c>
       <c r="B69" t="s">
         <v>1136</v>
@@ -6647,7 +6770,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="31">
-        <v>5.7540046296296294</v>
+        <v>5.7542476851851854</v>
       </c>
       <c r="B70" t="s">
         <v>1137</v>
@@ -6660,7 +6783,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="31">
-        <v>5.7546412037037031</v>
+        <v>5.7546527777777783</v>
       </c>
       <c r="B71" t="s">
         <v>1132</v>
@@ -6673,7 +6796,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="31">
-        <v>5.7546643518518517</v>
+        <v>5.7546759259259259</v>
       </c>
       <c r="B72" t="s">
         <v>1133</v>
@@ -7223,7 +7346,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="31">
-        <v>5.8959722222222224</v>
+        <v>5.8959606481481481</v>
       </c>
       <c r="B114" t="s">
         <v>823</v>
@@ -7236,7 +7359,7 @@
     </row>
     <row r="115" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="31">
-        <v>5.8959953703703709</v>
+        <v>5.8959837962962958</v>
       </c>
       <c r="B115" t="s">
         <v>824</v>
@@ -7250,7 +7373,7 @@
     </row>
     <row r="116" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="31">
-        <v>5.8960069444444443</v>
+        <v>5.8959953703703709</v>
       </c>
       <c r="B116" t="s">
         <v>825</v>
@@ -7264,7 +7387,7 @@
     </row>
     <row r="117" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="31">
-        <v>5.8960185185185177</v>
+        <v>5.8960069444444443</v>
       </c>
       <c r="B117" t="s">
         <v>826</v>
@@ -7278,7 +7401,7 @@
     </row>
     <row r="118" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="31">
-        <v>5.896076388888889</v>
+        <v>5.8960532407407413</v>
       </c>
       <c r="B118" t="s">
         <v>827</v>
@@ -7292,7 +7415,7 @@
     </row>
     <row r="119" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="31">
-        <v>5.8960879629629632</v>
+        <v>5.8960648148148147</v>
       </c>
       <c r="B119" t="s">
         <v>828</v>
@@ -7306,7 +7429,7 @@
     </row>
     <row r="120" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="31">
-        <v>5.8960995370370375</v>
+        <v>5.896076388888889</v>
       </c>
       <c r="B120" t="s">
         <v>829</v>
@@ -7320,7 +7443,7 @@
     </row>
     <row r="121" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="31">
-        <v>5.8962499999999993</v>
+        <v>5.8961805555555555</v>
       </c>
       <c r="B121" t="s">
         <v>830</v>
@@ -7334,7 +7457,7 @@
     </row>
     <row r="122" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="31">
-        <v>5.8962615740740745</v>
+        <v>5.8961921296296298</v>
       </c>
       <c r="B122" t="s">
         <v>831</v>
@@ -7348,7 +7471,7 @@
     </row>
     <row r="123" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="31">
-        <v>5.8962731481481478</v>
+        <v>5.8962037037037041</v>
       </c>
       <c r="B123" t="s">
         <v>832</v>
@@ -7362,7 +7485,7 @@
     </row>
     <row r="124" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="31">
-        <v>5.8962962962962964</v>
+        <v>5.8962152777777774</v>
       </c>
       <c r="B124" t="s">
         <v>833</v>
@@ -7488,7 +7611,7 @@
     </row>
     <row r="133" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>22</v>
+        <v>1725</v>
       </c>
       <c r="B133" t="s">
         <v>283</v>
@@ -7502,7 +7625,7 @@
     </row>
     <row r="134" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>23</v>
+        <v>1726</v>
       </c>
       <c r="B134" t="s">
         <v>284</v>
@@ -7516,7 +7639,7 @@
     </row>
     <row r="135" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>24</v>
+        <v>1727</v>
       </c>
       <c r="B135" t="s">
         <v>285</v>
@@ -7530,7 +7653,7 @@
     </row>
     <row r="136" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>25</v>
+        <v>1728</v>
       </c>
       <c r="B136" t="s">
         <v>286</v>
@@ -7544,7 +7667,7 @@
     </row>
     <row r="137" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>26</v>
+        <v>1729</v>
       </c>
       <c r="B137" t="s">
         <v>287</v>
@@ -7558,7 +7681,7 @@
     </row>
     <row r="138" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>27</v>
+        <v>1730</v>
       </c>
       <c r="B138" t="s">
         <v>288</v>
@@ -7572,7 +7695,7 @@
     </row>
     <row r="139" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>28</v>
+        <v>1731</v>
       </c>
       <c r="B139" t="s">
         <v>289</v>
@@ -7586,7 +7709,7 @@
     </row>
     <row r="140" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>29</v>
+        <v>1732</v>
       </c>
       <c r="B140" t="s">
         <v>290</v>
@@ -7600,7 +7723,7 @@
     </row>
     <row r="141" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>1383</v>
+        <v>1733</v>
       </c>
       <c r="B141" t="s">
         <v>291</v>
@@ -9120,7 +9243,7 @@
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
-        <v>1429</v>
+        <v>1734</v>
       </c>
       <c r="B254" t="s">
         <v>605</v>
@@ -9133,7 +9256,7 @@
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="s">
-        <v>1430</v>
+        <v>1735</v>
       </c>
       <c r="B255" t="s">
         <v>606</v>
@@ -9146,7 +9269,7 @@
     </row>
     <row r="256" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A256" s="3" t="s">
-        <v>1431</v>
+        <v>1736</v>
       </c>
       <c r="B256" t="s">
         <v>607</v>
@@ -9161,7 +9284,7 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
-        <v>1432</v>
+        <v>1737</v>
       </c>
       <c r="B257" t="s">
         <v>608</v>
@@ -9174,7 +9297,7 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="s">
-        <v>1433</v>
+        <v>1738</v>
       </c>
       <c r="B258" t="s">
         <v>609</v>
@@ -9187,7 +9310,7 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="s">
-        <v>1434</v>
+        <v>1739</v>
       </c>
       <c r="B259" t="s">
         <v>610</v>
@@ -9317,7 +9440,7 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="3" t="s">
-        <v>83</v>
+        <v>1740</v>
       </c>
       <c r="B269" t="s">
         <v>624</v>
@@ -9330,7 +9453,7 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="3" t="s">
-        <v>84</v>
+        <v>1741</v>
       </c>
       <c r="B270" t="s">
         <v>625</v>
@@ -9343,7 +9466,7 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="s">
-        <v>85</v>
+        <v>1742</v>
       </c>
       <c r="B271" t="s">
         <v>626</v>
@@ -9356,7 +9479,7 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="3" t="s">
-        <v>86</v>
+        <v>1743</v>
       </c>
       <c r="B272" t="s">
         <v>627</v>
@@ -9434,7 +9557,7 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="3" t="s">
-        <v>225</v>
+        <v>1744</v>
       </c>
       <c r="B278" t="s">
         <v>673</v>
@@ -9447,7 +9570,7 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="3" t="s">
-        <v>226</v>
+        <v>1745</v>
       </c>
       <c r="B279" t="s">
         <v>674</v>
@@ -10149,7 +10272,7 @@
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A333" s="26" t="s">
-        <v>1476</v>
+        <v>1640</v>
       </c>
       <c r="B333" s="22" t="s">
         <v>477</v>
@@ -10162,7 +10285,7 @@
     </row>
     <row r="334" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A334" s="26" t="s">
-        <v>1477</v>
+        <v>1641</v>
       </c>
       <c r="B334" s="22" t="s">
         <v>478</v>
@@ -10175,7 +10298,7 @@
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A335" s="26" t="s">
-        <v>1478</v>
+        <v>1642</v>
       </c>
       <c r="B335" s="22" t="s">
         <v>479</v>
@@ -10188,7 +10311,7 @@
     </row>
     <row r="336" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A336" s="26" t="s">
-        <v>1479</v>
+        <v>1643</v>
       </c>
       <c r="B336" s="22" t="s">
         <v>481</v>
@@ -10203,7 +10326,7 @@
     </row>
     <row r="337" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A337" s="26" t="s">
-        <v>1480</v>
+        <v>1644</v>
       </c>
       <c r="B337" s="22" t="s">
         <v>482</v>
@@ -10216,7 +10339,7 @@
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A338" s="26" t="s">
-        <v>1481</v>
+        <v>1645</v>
       </c>
       <c r="B338" s="22" t="s">
         <v>483</v>
@@ -10229,7 +10352,7 @@
     </row>
     <row r="339" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A339" s="26" t="s">
-        <v>1482</v>
+        <v>1646</v>
       </c>
       <c r="B339" s="22" t="s">
         <v>484</v>
@@ -10244,7 +10367,7 @@
     </row>
     <row r="340" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A340" s="26" t="s">
-        <v>1483</v>
+        <v>1647</v>
       </c>
       <c r="B340" s="22" t="s">
         <v>485</v>
@@ -10257,7 +10380,7 @@
     </row>
     <row r="341" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A341" s="3" t="s">
-        <v>1640</v>
+        <v>1648</v>
       </c>
       <c r="B341" t="s">
         <v>486</v>
@@ -10272,7 +10395,7 @@
     </row>
     <row r="342" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A342" s="3" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
       <c r="B342" t="s">
         <v>488</v>
@@ -10285,7 +10408,7 @@
     </row>
     <row r="343" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A343" s="3" t="s">
-        <v>1642</v>
+        <v>1650</v>
       </c>
       <c r="B343" t="s">
         <v>489</v>
@@ -10300,7 +10423,7 @@
     </row>
     <row r="344" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A344" s="3" t="s">
-        <v>1643</v>
+        <v>1651</v>
       </c>
       <c r="B344" t="s">
         <v>490</v>
@@ -10313,7 +10436,7 @@
     </row>
     <row r="345" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="s">
-        <v>1644</v>
+        <v>1652</v>
       </c>
       <c r="B345" t="s">
         <v>491</v>
@@ -10326,7 +10449,7 @@
     </row>
     <row r="346" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A346" s="3" t="s">
-        <v>1645</v>
+        <v>1653</v>
       </c>
       <c r="B346" t="s">
         <v>492</v>
@@ -10341,7 +10464,7 @@
     </row>
     <row r="347" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A347" s="3" t="s">
-        <v>1646</v>
+        <v>1654</v>
       </c>
       <c r="B347" t="s">
         <v>493</v>
@@ -10354,7 +10477,7 @@
     </row>
     <row r="348" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A348" s="3" t="s">
-        <v>1647</v>
+        <v>1655</v>
       </c>
       <c r="B348" t="s">
         <v>494</v>
@@ -10367,7 +10490,7 @@
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" s="3" t="s">
-        <v>1648</v>
+        <v>1656</v>
       </c>
       <c r="B349" t="s">
         <v>495</v>
@@ -10380,7 +10503,7 @@
     </row>
     <row r="350" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
-        <v>1649</v>
+        <v>1657</v>
       </c>
       <c r="B350" t="s">
         <v>496</v>
@@ -10395,7 +10518,7 @@
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
-        <v>1650</v>
+        <v>1658</v>
       </c>
       <c r="B351" t="s">
         <v>497</v>
@@ -10408,7 +10531,7 @@
     </row>
     <row r="352" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A352" s="3" t="s">
-        <v>1651</v>
+        <v>1659</v>
       </c>
       <c r="B352" t="s">
         <v>498</v>
@@ -10423,7 +10546,7 @@
     </row>
     <row r="353" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A353" s="3" t="s">
-        <v>1652</v>
+        <v>1660</v>
       </c>
       <c r="B353" t="s">
         <v>499</v>
@@ -10438,7 +10561,7 @@
     </row>
     <row r="354" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A354" s="3" t="s">
-        <v>1653</v>
+        <v>1661</v>
       </c>
       <c r="B354" t="s">
         <v>500</v>
@@ -10453,7 +10576,7 @@
     </row>
     <row r="355" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A355" s="3" t="s">
-        <v>1654</v>
+        <v>1662</v>
       </c>
       <c r="B355" t="s">
         <v>501</v>
@@ -10468,7 +10591,7 @@
     </row>
     <row r="356" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A356" s="3" t="s">
-        <v>1655</v>
+        <v>1663</v>
       </c>
       <c r="B356" t="s">
         <v>502</v>
@@ -10483,7 +10606,7 @@
     </row>
     <row r="357" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A357" s="3" t="s">
-        <v>1656</v>
+        <v>1664</v>
       </c>
       <c r="B357" t="s">
         <v>503</v>
@@ -10498,7 +10621,7 @@
     </row>
     <row r="358" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A358" s="3" t="s">
-        <v>1657</v>
+        <v>1515</v>
       </c>
       <c r="B358" t="s">
         <v>504</v>
@@ -10513,7 +10636,7 @@
     </row>
     <row r="359" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A359" s="3" t="s">
-        <v>1658</v>
+        <v>1665</v>
       </c>
       <c r="B359" t="s">
         <v>505</v>
@@ -10528,7 +10651,7 @@
     </row>
     <row r="360" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A360" s="3" t="s">
-        <v>1659</v>
+        <v>1666</v>
       </c>
       <c r="B360" t="s">
         <v>506</v>
@@ -10543,7 +10666,7 @@
     </row>
     <row r="361" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A361" s="3" t="s">
-        <v>1660</v>
+        <v>1667</v>
       </c>
       <c r="B361" t="s">
         <v>507</v>
@@ -10558,7 +10681,7 @@
     </row>
     <row r="362" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A362" s="3" t="s">
-        <v>1661</v>
+        <v>1514</v>
       </c>
       <c r="B362" t="s">
         <v>508</v>
@@ -10573,7 +10696,7 @@
     </row>
     <row r="363" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A363" s="3" t="s">
-        <v>1662</v>
+        <v>1668</v>
       </c>
       <c r="B363" t="s">
         <v>509</v>
@@ -10588,7 +10711,7 @@
     </row>
     <row r="364" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A364" s="3" t="s">
-        <v>1663</v>
+        <v>1669</v>
       </c>
       <c r="B364" t="s">
         <v>510</v>
@@ -10603,7 +10726,7 @@
     </row>
     <row r="365" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A365" s="3" t="s">
-        <v>1664</v>
+        <v>1670</v>
       </c>
       <c r="B365" t="s">
         <v>511</v>
@@ -10616,7 +10739,7 @@
     </row>
     <row r="366" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A366" s="3" t="s">
-        <v>1515</v>
+        <v>1671</v>
       </c>
       <c r="B366" t="s">
         <v>512</v>
@@ -10631,7 +10754,7 @@
     </row>
     <row r="367" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A367" s="3" t="s">
-        <v>1665</v>
+        <v>1672</v>
       </c>
       <c r="B367" t="s">
         <v>513</v>
@@ -10644,7 +10767,7 @@
     </row>
     <row r="368" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A368" s="3" t="s">
-        <v>1666</v>
+        <v>1673</v>
       </c>
       <c r="B368" t="s">
         <v>514</v>
@@ -10657,7 +10780,7 @@
     </row>
     <row r="369" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A369" s="3" t="s">
-        <v>1667</v>
+        <v>1674</v>
       </c>
       <c r="B369" t="s">
         <v>515</v>
@@ -10672,7 +10795,7 @@
     </row>
     <row r="370" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A370" s="3" t="s">
-        <v>1514</v>
+        <v>1675</v>
       </c>
       <c r="B370" t="s">
         <v>516</v>
@@ -10687,7 +10810,7 @@
     </row>
     <row r="371" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A371" s="3" t="s">
-        <v>1668</v>
+        <v>1676</v>
       </c>
       <c r="B371" t="s">
         <v>517</v>
@@ -10700,7 +10823,7 @@
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372" s="3" t="s">
-        <v>1669</v>
+        <v>1677</v>
       </c>
       <c r="B372" t="s">
         <v>518</v>
@@ -10713,7 +10836,7 @@
     </row>
     <row r="373" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A373" s="3" t="s">
-        <v>1670</v>
+        <v>1678</v>
       </c>
       <c r="B373" t="s">
         <v>519</v>
@@ -10726,7 +10849,7 @@
     </row>
     <row r="374" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A374" s="3" t="s">
-        <v>1671</v>
+        <v>1679</v>
       </c>
       <c r="B374" t="s">
         <v>520</v>
@@ -10741,7 +10864,7 @@
     </row>
     <row r="375" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A375" s="3" t="s">
-        <v>1672</v>
+        <v>1680</v>
       </c>
       <c r="B375" t="s">
         <v>521</v>
@@ -10756,7 +10879,7 @@
     </row>
     <row r="376" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A376" s="3" t="s">
-        <v>1673</v>
+        <v>1681</v>
       </c>
       <c r="B376" t="s">
         <v>522</v>
@@ -10771,7 +10894,7 @@
     </row>
     <row r="377" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="3" t="s">
-        <v>1674</v>
+        <v>1682</v>
       </c>
       <c r="B377" t="s">
         <v>523</v>
@@ -10786,7 +10909,7 @@
     </row>
     <row r="378" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A378" s="3" t="s">
-        <v>1675</v>
+        <v>1683</v>
       </c>
       <c r="B378" t="s">
         <v>524</v>
@@ -10801,7 +10924,7 @@
     </row>
     <row r="379" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A379" s="3" t="s">
-        <v>1676</v>
+        <v>1684</v>
       </c>
       <c r="B379" t="s">
         <v>525</v>
@@ -10816,7 +10939,7 @@
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A380" s="3" t="s">
-        <v>1677</v>
+        <v>1685</v>
       </c>
       <c r="B380" t="s">
         <v>526</v>
@@ -10829,7 +10952,7 @@
     </row>
     <row r="381" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A381" s="3" t="s">
-        <v>1678</v>
+        <v>1686</v>
       </c>
       <c r="B381" t="s">
         <v>527</v>
@@ -10842,7 +10965,7 @@
     </row>
     <row r="382" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A382" s="3" t="s">
-        <v>1679</v>
+        <v>1687</v>
       </c>
       <c r="B382" t="s">
         <v>528</v>
@@ -10855,7 +10978,7 @@
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A383" s="3" t="s">
-        <v>1680</v>
+        <v>1688</v>
       </c>
       <c r="B383" t="s">
         <v>529</v>
@@ -10868,7 +10991,7 @@
     </row>
     <row r="384" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A384" s="3" t="s">
-        <v>1681</v>
+        <v>1689</v>
       </c>
       <c r="B384" t="s">
         <v>530</v>
@@ -10883,7 +11006,7 @@
     </row>
     <row r="385" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A385" s="3" t="s">
-        <v>1682</v>
+        <v>1690</v>
       </c>
       <c r="B385" t="s">
         <v>531</v>
@@ -10898,7 +11021,7 @@
     </row>
     <row r="386" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A386" s="3" t="s">
-        <v>1683</v>
+        <v>1691</v>
       </c>
       <c r="B386" t="s">
         <v>532</v>
@@ -10913,7 +11036,7 @@
     </row>
     <row r="387" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A387" s="3" t="s">
-        <v>1684</v>
+        <v>1692</v>
       </c>
       <c r="B387" t="s">
         <v>533</v>
@@ -10928,7 +11051,7 @@
     </row>
     <row r="388" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A388" s="3" t="s">
-        <v>1685</v>
+        <v>1693</v>
       </c>
       <c r="B388" t="s">
         <v>534</v>
@@ -10943,7 +11066,7 @@
     </row>
     <row r="389" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A389" s="3" t="s">
-        <v>1686</v>
+        <v>1694</v>
       </c>
       <c r="B389" t="s">
         <v>535</v>
@@ -10958,7 +11081,7 @@
     </row>
     <row r="390" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A390" s="3" t="s">
-        <v>1687</v>
+        <v>1695</v>
       </c>
       <c r="B390" t="s">
         <v>536</v>
@@ -10973,7 +11096,7 @@
     </row>
     <row r="391" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A391" s="3" t="s">
-        <v>1688</v>
+        <v>1696</v>
       </c>
       <c r="B391" t="s">
         <v>537</v>
@@ -10988,7 +11111,7 @@
     </row>
     <row r="392" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A392" s="3" t="s">
-        <v>1689</v>
+        <v>1697</v>
       </c>
       <c r="B392" t="s">
         <v>538</v>
@@ -11004,7 +11127,7 @@
     </row>
     <row r="393" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A393" s="3" t="s">
-        <v>1690</v>
+        <v>1698</v>
       </c>
       <c r="B393" t="s">
         <v>539</v>
@@ -11019,7 +11142,7 @@
     </row>
     <row r="394" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A394" s="3" t="s">
-        <v>1691</v>
+        <v>1746</v>
       </c>
       <c r="B394" t="s">
         <v>540</v>
@@ -11034,7 +11157,7 @@
     </row>
     <row r="395" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A395" s="3" t="s">
-        <v>1692</v>
+        <v>1747</v>
       </c>
       <c r="B395" t="s">
         <v>541</v>
@@ -11049,7 +11172,7 @@
     </row>
     <row r="396" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A396" s="3" t="s">
-        <v>1693</v>
+        <v>1748</v>
       </c>
       <c r="B396" t="s">
         <v>542</v>
@@ -11064,7 +11187,7 @@
     </row>
     <row r="397" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A397" s="3" t="s">
-        <v>1694</v>
+        <v>1749</v>
       </c>
       <c r="B397" t="s">
         <v>543</v>
@@ -11077,7 +11200,7 @@
     </row>
     <row r="398" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A398" s="3" t="s">
-        <v>1695</v>
+        <v>1750</v>
       </c>
       <c r="B398" t="s">
         <v>544</v>
@@ -11090,7 +11213,7 @@
     </row>
     <row r="399" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A399" s="3" t="s">
-        <v>1696</v>
+        <v>1704</v>
       </c>
       <c r="B399" t="s">
         <v>545</v>
@@ -11103,7 +11226,7 @@
     </row>
     <row r="400" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A400" s="3" t="s">
-        <v>1697</v>
+        <v>1705</v>
       </c>
       <c r="B400" t="s">
         <v>546</v>
@@ -11116,7 +11239,7 @@
     </row>
     <row r="401" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A401" s="3" t="s">
-        <v>1698</v>
+        <v>1706</v>
       </c>
       <c r="B401" t="s">
         <v>547</v>
@@ -11129,7 +11252,7 @@
     </row>
     <row r="402" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A402" s="3" t="s">
-        <v>1699</v>
+        <v>1707</v>
       </c>
       <c r="B402" t="s">
         <v>548</v>
@@ -11142,7 +11265,7 @@
     </row>
     <row r="403" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A403" s="3" t="s">
-        <v>1700</v>
+        <v>1708</v>
       </c>
       <c r="B403" t="s">
         <v>549</v>
@@ -11155,7 +11278,7 @@
     </row>
     <row r="404" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A404" s="3" t="s">
-        <v>1701</v>
+        <v>1709</v>
       </c>
       <c r="B404" t="s">
         <v>550</v>
@@ -11168,7 +11291,7 @@
     </row>
     <row r="405" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A405" s="3" t="s">
-        <v>1702</v>
+        <v>1710</v>
       </c>
       <c r="B405" t="s">
         <v>551</v>
@@ -11181,7 +11304,7 @@
     </row>
     <row r="406" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A406" s="3" t="s">
-        <v>1703</v>
+        <v>1711</v>
       </c>
       <c r="B406" t="s">
         <v>552</v>
@@ -11196,7 +11319,7 @@
     </row>
     <row r="407" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A407" s="3" t="s">
-        <v>1704</v>
+        <v>1712</v>
       </c>
       <c r="B407" t="s">
         <v>553</v>
@@ -11211,7 +11334,7 @@
     </row>
     <row r="408" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A408" s="3" t="s">
-        <v>1705</v>
+        <v>1713</v>
       </c>
       <c r="B408" t="s">
         <v>554</v>
@@ -11226,7 +11349,7 @@
     </row>
     <row r="409" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A409" s="3" t="s">
-        <v>1706</v>
+        <v>1714</v>
       </c>
       <c r="B409" t="s">
         <v>555</v>
@@ -11240,7 +11363,7 @@
     </row>
     <row r="410" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A410" s="3" t="s">
-        <v>1707</v>
+        <v>1715</v>
       </c>
       <c r="B410" t="s">
         <v>556</v>
@@ -11254,7 +11377,7 @@
     </row>
     <row r="411" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A411" s="3" t="s">
-        <v>1708</v>
+        <v>1716</v>
       </c>
       <c r="B411" t="s">
         <v>557</v>
@@ -11267,7 +11390,7 @@
     </row>
     <row r="412" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A412" s="3" t="s">
-        <v>1709</v>
+        <v>1717</v>
       </c>
       <c r="B412" t="s">
         <v>558</v>
@@ -11280,7 +11403,7 @@
     </row>
     <row r="413" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A413" s="3" t="s">
-        <v>1710</v>
+        <v>1718</v>
       </c>
       <c r="B413" t="s">
         <v>559</v>
@@ -11293,7 +11416,7 @@
     </row>
     <row r="414" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A414" s="3" t="s">
-        <v>1711</v>
+        <v>1719</v>
       </c>
       <c r="B414" t="s">
         <v>560</v>
@@ -11306,7 +11429,7 @@
     </row>
     <row r="415" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A415" s="3" t="s">
-        <v>1712</v>
+        <v>1720</v>
       </c>
       <c r="B415" t="s">
         <v>561</v>
@@ -11319,7 +11442,7 @@
     </row>
     <row r="416" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A416" s="3" t="s">
-        <v>1713</v>
+        <v>1721</v>
       </c>
       <c r="B416" t="s">
         <v>562</v>
@@ -11332,7 +11455,7 @@
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A417" s="3" t="s">
-        <v>1714</v>
+        <v>1751</v>
       </c>
       <c r="B417" t="s">
         <v>563</v>
@@ -11345,7 +11468,7 @@
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A418" s="3" t="s">
-        <v>1715</v>
+        <v>1752</v>
       </c>
       <c r="B418" t="s">
         <v>564</v>
@@ -11358,7 +11481,7 @@
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A419" s="3" t="s">
-        <v>1716</v>
+        <v>1753</v>
       </c>
       <c r="B419" t="s">
         <v>565</v>
@@ -11371,7 +11494,7 @@
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A420" s="3" t="s">
-        <v>1717</v>
+        <v>1754</v>
       </c>
       <c r="B420" t="s">
         <v>566</v>
@@ -11384,7 +11507,7 @@
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A421" s="3" t="s">
-        <v>1718</v>
+        <v>1755</v>
       </c>
       <c r="B421" t="s">
         <v>568</v>
@@ -11397,7 +11520,7 @@
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A422" s="3" t="s">
-        <v>1719</v>
+        <v>1756</v>
       </c>
       <c r="B422" t="s">
         <v>569</v>
@@ -11410,7 +11533,7 @@
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A423" s="3" t="s">
-        <v>1720</v>
+        <v>1757</v>
       </c>
       <c r="B423" t="s">
         <v>571</v>
@@ -11423,7 +11546,7 @@
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A424" s="3" t="s">
-        <v>1721</v>
+        <v>1577</v>
       </c>
       <c r="B424" t="s">
         <v>573</v>
@@ -11436,7 +11559,7 @@
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A425" s="3" t="s">
-        <v>1722</v>
+        <v>1578</v>
       </c>
       <c r="B425" t="s">
         <v>575</v>
@@ -11449,7 +11572,7 @@
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A426" s="3" t="s">
-        <v>1723</v>
+        <v>1579</v>
       </c>
       <c r="B426" t="s">
         <v>576</v>
@@ -11462,7 +11585,7 @@
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A427" s="3" t="s">
-        <v>1570</v>
+        <v>1580</v>
       </c>
       <c r="B427" t="s">
         <v>578</v>
@@ -11475,7 +11598,7 @@
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428" s="26" t="s">
-        <v>1571</v>
+        <v>1581</v>
       </c>
       <c r="B428" s="22" t="s">
         <v>579</v>
@@ -11488,7 +11611,7 @@
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A429" s="26" t="s">
-        <v>1572</v>
+        <v>1582</v>
       </c>
       <c r="B429" s="22" t="s">
         <v>580</v>
@@ -11501,7 +11624,7 @@
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A430" s="3" t="s">
-        <v>1573</v>
+        <v>1583</v>
       </c>
       <c r="B430" t="s">
         <v>582</v>
@@ -11514,7 +11637,7 @@
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A431" s="3" t="s">
-        <v>1574</v>
+        <v>266</v>
       </c>
       <c r="B431" t="s">
         <v>596</v>
@@ -11527,7 +11650,7 @@
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A432" s="3" t="s">
-        <v>1575</v>
+        <v>267</v>
       </c>
       <c r="B432" t="s">
         <v>598</v>
@@ -11540,7 +11663,7 @@
     </row>
     <row r="433" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A433" s="3" t="s">
-        <v>1576</v>
+        <v>1584</v>
       </c>
       <c r="B433" t="s">
         <v>599</v>
@@ -11553,7 +11676,7 @@
     </row>
     <row r="434" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A434" s="3" t="s">
-        <v>1577</v>
+        <v>1585</v>
       </c>
       <c r="B434" t="s">
         <v>602</v>
@@ -11566,7 +11689,7 @@
     </row>
     <row r="435" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A435" s="3" t="s">
-        <v>1578</v>
+        <v>1586</v>
       </c>
       <c r="B435" t="s">
         <v>603</v>
@@ -11579,7 +11702,7 @@
     </row>
     <row r="436" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A436" s="3" t="s">
-        <v>1579</v>
+        <v>1587</v>
       </c>
       <c r="B436" t="s">
         <v>604</v>
@@ -11763,7 +11886,7 @@
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A450" s="3" t="s">
-        <v>1009</v>
+        <v>1758</v>
       </c>
       <c r="B450" t="s">
         <v>310</v>
@@ -11841,7 +11964,7 @@
     </row>
     <row r="456" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A456" s="3" t="s">
-        <v>1010</v>
+        <v>1759</v>
       </c>
       <c r="B456" t="s">
         <v>316</v>
@@ -12361,7 +12484,7 @@
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A496" s="3" t="s">
-        <v>1015</v>
+        <v>1760</v>
       </c>
       <c r="B496" t="s">
         <v>635</v>
@@ -12374,7 +12497,7 @@
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A497" s="3" t="s">
-        <v>1016</v>
+        <v>1761</v>
       </c>
       <c r="B497" t="s">
         <v>636</v>
@@ -12737,8 +12860,8 @@
       </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A525" s="31">
-        <v>4.1857754629629627</v>
+      <c r="A525" s="31" t="s">
+        <v>1762</v>
       </c>
       <c r="B525" t="s">
         <v>675</v>
@@ -12750,8 +12873,8 @@
       </c>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A526" s="31">
-        <v>4.1859606481481482</v>
+      <c r="A526" s="31" t="s">
+        <v>1763</v>
       </c>
       <c r="B526" t="s">
         <v>676</v>
@@ -12763,8 +12886,8 @@
       </c>
     </row>
     <row r="527" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A527" s="31">
-        <v>4.1862962962962964</v>
+      <c r="A527" s="31" t="s">
+        <v>1764</v>
       </c>
       <c r="B527" t="s">
         <v>677</v>
@@ -12776,8 +12899,8 @@
       </c>
     </row>
     <row r="528" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A528" s="31">
-        <v>4.1919097222222224</v>
+      <c r="A528" s="31" t="s">
+        <v>1765</v>
       </c>
       <c r="B528" t="s">
         <v>678</v>
@@ -12790,7 +12913,7 @@
     </row>
     <row r="529" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A529" s="31">
-        <v>4.1992476851851857</v>
+        <v>4.2048032407407403</v>
       </c>
       <c r="B529" t="s">
         <v>679</v>
@@ -12803,7 +12926,7 @@
     </row>
     <row r="530" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A530" s="31">
-        <v>4.1994791666666664</v>
+        <v>4.205034722222222</v>
       </c>
       <c r="B530" t="s">
         <v>680</v>
@@ -12816,7 +12939,7 @@
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A531" s="31">
-        <v>4.1997106481481481</v>
+        <v>4.2052777777777779</v>
       </c>
       <c r="B531" t="s">
         <v>681</v>
@@ -12868,7 +12991,7 @@
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A535" s="31">
-        <v>4.2558449074074076</v>
+        <v>4.2614004629629632</v>
       </c>
       <c r="B535" t="s">
         <v>685</v>
@@ -12881,7 +13004,7 @@
     </row>
     <row r="536" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A536" s="31">
-        <v>4.2560763888888884</v>
+        <v>4.2616435185185191</v>
       </c>
       <c r="B536" t="s">
         <v>686</v>
@@ -12894,7 +13017,7 @@
     </row>
     <row r="537" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A537" s="31">
-        <v>4.2563194444444443</v>
+        <v>4.2618749999999999</v>
       </c>
       <c r="B537" t="s">
         <v>687</v>
@@ -12907,7 +13030,7 @@
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A538" s="31">
-        <v>4.2565277777777775</v>
+        <v>4.2620833333333339</v>
       </c>
       <c r="B538" t="s">
         <v>688</v>
@@ -12920,7 +13043,7 @@
     </row>
     <row r="539" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A539" s="31">
-        <v>4.2567939814814819</v>
+        <v>4.2623495370370366</v>
       </c>
       <c r="B539" t="s">
         <v>689</v>
@@ -12933,7 +13056,7 @@
     </row>
     <row r="540" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A540" s="31">
-        <v>4.2571064814814816</v>
+        <v>4.2626620370370372</v>
       </c>
       <c r="B540" t="s">
         <v>690</v>
@@ -12946,7 +13069,7 @@
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A541" s="31">
-        <v>4.2572106481481482</v>
+        <v>4.2627662037037037</v>
       </c>
       <c r="B541" t="s">
         <v>691</v>
@@ -12959,7 +13082,7 @@
     </row>
     <row r="542" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A542" s="31">
-        <v>4.2578472222222219</v>
+        <v>4.2634027777777783</v>
       </c>
       <c r="B542" t="s">
         <v>692</v>
@@ -12972,7 +13095,7 @@
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A543" s="31">
-        <v>4.2593865740740737</v>
+        <v>4.2649421296296302</v>
       </c>
       <c r="B543" t="s">
         <v>693</v>
@@ -12985,7 +13108,7 @@
     </row>
     <row r="544" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A544" s="31">
-        <v>4.2629166666666665</v>
+        <v>4.2675925925925924</v>
       </c>
       <c r="B544" t="s">
         <v>694</v>
@@ -13779,7 +13902,7 @@
     </row>
     <row r="605" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A605" s="31">
-        <v>5.0167129629629628</v>
+        <v>5.0136805555555553</v>
       </c>
       <c r="B605" t="s">
         <v>755</v>
@@ -13792,7 +13915,7 @@
     </row>
     <row r="606" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A606" s="31">
-        <v>5.0179513888888891</v>
+        <v>5.0139467592592597</v>
       </c>
       <c r="B606" t="s">
         <v>756</v>

</xml_diff>

<commit_message>
Added graph overlay Added GET jump text element and button
</commit_message>
<xml_diff>
--- a/MISSION_DATA/A13_photos.xlsx
+++ b/MISSION_DATA/A13_photos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apollo_13\MISSION_DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27B2728-8D73-47B9-B3A6-B28D41AC349B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A331F70-DE2C-4843-B328-B7878380191A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10500" yWindow="4260" windowWidth="38535" windowHeight="23985" xr2:uid="{E7285D04-3DFB-428F-BD58-901528569A82}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4660" uniqueCount="1698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4660" uniqueCount="1798">
   <si>
     <t>LM &amp; S-IVB during Transposition and Docking</t>
   </si>
@@ -5032,136 +5032,436 @@
     <t>138:11:41</t>
   </si>
   <si>
+    <t>138:11:50</t>
+  </si>
+  <si>
+    <t>138:12:01</t>
+  </si>
+  <si>
+    <t>138:12:03</t>
+  </si>
+  <si>
+    <t>138:12:06</t>
+  </si>
+  <si>
+    <t>141:29:47</t>
+  </si>
+  <si>
+    <t>141:29:51</t>
+  </si>
+  <si>
+    <t>141:29:53</t>
+  </si>
+  <si>
+    <t>141:29:56</t>
+  </si>
+  <si>
+    <t>141:29:57</t>
+  </si>
+  <si>
+    <t>141:29:59</t>
+  </si>
+  <si>
+    <t>141:30:08</t>
+  </si>
+  <si>
+    <t>141:30:10</t>
+  </si>
+  <si>
+    <t>141:30:12</t>
+  </si>
+  <si>
+    <t>141:30:16</t>
+  </si>
+  <si>
+    <t>141:30:17</t>
+  </si>
+  <si>
+    <t>141:30:18</t>
+  </si>
+  <si>
+    <t>141:30:24</t>
+  </si>
+  <si>
+    <t>141:30:25</t>
+  </si>
+  <si>
+    <t>141:30:26</t>
+  </si>
+  <si>
+    <t>141:30:27</t>
+  </si>
+  <si>
+    <t>009:03:13</t>
+  </si>
+  <si>
+    <t>009:26:36</t>
+  </si>
+  <si>
+    <t>095:50:49</t>
+  </si>
+  <si>
+    <t>095:51:01</t>
+  </si>
+  <si>
+    <t>095:52:38</t>
+  </si>
+  <si>
+    <t>094:15:02</t>
+  </si>
+  <si>
+    <t>094:15:48</t>
+  </si>
+  <si>
+    <t>078:02:15</t>
+  </si>
+  <si>
+    <t>087:47:15</t>
+  </si>
+  <si>
+    <t>087:47:27</t>
+  </si>
+  <si>
+    <t>100:47:16</t>
+  </si>
+  <si>
+    <t>100:49:48</t>
+  </si>
+  <si>
+    <t>104:45:58</t>
+  </si>
+  <si>
+    <t>104:46:20</t>
+  </si>
+  <si>
+    <t>091:02:15</t>
+  </si>
+  <si>
+    <t>091:44:40</t>
+  </si>
+  <si>
+    <t>091:44:56</t>
+  </si>
+  <si>
+    <t>091:32:54</t>
+  </si>
+  <si>
+    <t>075:17:21</t>
+  </si>
+  <si>
+    <t>075:17:35</t>
+  </si>
+  <si>
+    <t>075:17:47</t>
+  </si>
+  <si>
+    <t>075:18:02</t>
+  </si>
+  <si>
+    <t>097:18:58</t>
+  </si>
+  <si>
+    <t>104:57:21</t>
+  </si>
+  <si>
+    <t>104:59:33</t>
+  </si>
+  <si>
+    <t>105:00:16</t>
+  </si>
+  <si>
+    <t>105:00:28</t>
+  </si>
+  <si>
+    <t>105:01:40</t>
+  </si>
+  <si>
+    <t>105:02:21</t>
+  </si>
+  <si>
+    <t>105:04:03</t>
+  </si>
+  <si>
+    <t>105:05:26</t>
+  </si>
+  <si>
+    <t>105:05:50</t>
+  </si>
+  <si>
+    <t>105:06:17</t>
+  </si>
+  <si>
+    <t>105:06:41</t>
+  </si>
+  <si>
+    <t>105:08:06</t>
+  </si>
+  <si>
+    <t>105:08:21</t>
+  </si>
+  <si>
+    <t>105:08:39</t>
+  </si>
+  <si>
+    <t>105:12:12</t>
+  </si>
+  <si>
+    <t>105:54:46</t>
+  </si>
+  <si>
+    <t>105:55:01</t>
+  </si>
+  <si>
+    <t>105:55:28</t>
+  </si>
+  <si>
+    <t>105:56:32</t>
+  </si>
+  <si>
+    <t>107:10:55</t>
+  </si>
+  <si>
+    <t>107:11:15</t>
+  </si>
+  <si>
+    <t>107:11:36</t>
+  </si>
+  <si>
+    <t>107:12:38</t>
+  </si>
+  <si>
+    <t>107:13:25</t>
+  </si>
+  <si>
+    <t>107:13:50</t>
+  </si>
+  <si>
+    <t>108:32:47</t>
+  </si>
+  <si>
+    <t>108:32:55</t>
+  </si>
+  <si>
+    <t>108:33:04</t>
+  </si>
+  <si>
+    <t>108:33:12</t>
+  </si>
+  <si>
+    <t>108:42:27</t>
+  </si>
+  <si>
+    <t>108:42:35</t>
+  </si>
+  <si>
+    <t>108:42:45</t>
+  </si>
+  <si>
+    <t>108:42:53</t>
+  </si>
+  <si>
+    <t>109:02:27</t>
+  </si>
+  <si>
+    <t>118:54:16</t>
+  </si>
+  <si>
+    <t>118:54:55</t>
+  </si>
+  <si>
+    <t>118:55:20</t>
+  </si>
+  <si>
+    <t>118:55:42</t>
+  </si>
+  <si>
+    <t>118:55:59</t>
+  </si>
+  <si>
+    <t>118:56:13</t>
+  </si>
+  <si>
+    <t>118:56:23</t>
+  </si>
+  <si>
+    <t>119:00:10</t>
+  </si>
+  <si>
+    <t>119:00:16</t>
+  </si>
+  <si>
+    <t>119:16:02</t>
+  </si>
+  <si>
+    <t>119:16:07</t>
+  </si>
+  <si>
+    <t>119:16:13</t>
+  </si>
+  <si>
+    <t>119:16:30</t>
+  </si>
+  <si>
+    <t>119:16:36</t>
+  </si>
+  <si>
+    <t>119:19:57</t>
+  </si>
+  <si>
+    <t>119:20:08</t>
+  </si>
+  <si>
+    <t>119:20:17</t>
+  </si>
+  <si>
+    <t>119:20:24</t>
+  </si>
+  <si>
+    <t>119:20:31</t>
+  </si>
+  <si>
+    <t>119:20:40</t>
+  </si>
+  <si>
+    <t>119:20:51</t>
+  </si>
+  <si>
+    <t>119:23:17</t>
+  </si>
+  <si>
+    <t>119:23:25</t>
+  </si>
+  <si>
+    <t>119:23:32</t>
+  </si>
+  <si>
+    <t>119:36:00</t>
+  </si>
+  <si>
+    <t>119:36:03</t>
+  </si>
+  <si>
+    <t>119:36:08</t>
+  </si>
+  <si>
+    <t>122:08:12</t>
+  </si>
+  <si>
+    <t>122:08:20</t>
+  </si>
+  <si>
+    <t>122:08:27</t>
+  </si>
+  <si>
+    <t>122:08:33</t>
+  </si>
+  <si>
+    <t>122:08:41</t>
+  </si>
+  <si>
+    <t>124:46:21</t>
+  </si>
+  <si>
+    <t>124:47:00</t>
+  </si>
+  <si>
+    <t>124:46:46</t>
+  </si>
+  <si>
+    <t>124:49:58</t>
+  </si>
+  <si>
+    <t>124:50:09</t>
+  </si>
+  <si>
+    <t>124:50:17</t>
+  </si>
+  <si>
+    <t>124:52:08</t>
+  </si>
+  <si>
+    <t>124:52:15</t>
+  </si>
+  <si>
+    <t>124:52:24</t>
+  </si>
+  <si>
+    <t>124:55:16</t>
+  </si>
+  <si>
+    <t>124:55:24</t>
+  </si>
+  <si>
+    <t>124:55:33</t>
+  </si>
+  <si>
+    <t>127:07:26</t>
+  </si>
+  <si>
+    <t>127:07:40</t>
+  </si>
+  <si>
+    <t>127:07:51</t>
+  </si>
+  <si>
+    <t>127:08:05</t>
+  </si>
+  <si>
+    <t>127:08:26</t>
+  </si>
+  <si>
+    <t>127:18:13</t>
+  </si>
+  <si>
+    <t>127:18:21</t>
+  </si>
+  <si>
+    <t>127:18:30</t>
+  </si>
+  <si>
+    <t>127:18:47</t>
+  </si>
+  <si>
+    <t>127:22:42</t>
+  </si>
+  <si>
+    <t>127:22:55</t>
+  </si>
+  <si>
+    <t>127:26:36</t>
+  </si>
+  <si>
+    <t>127:31:45</t>
+  </si>
+  <si>
+    <t>127:31:58</t>
+  </si>
+  <si>
+    <t>127:32:16</t>
+  </si>
+  <si>
+    <t>127:32:25</t>
+  </si>
+  <si>
+    <t>137:15:54</t>
+  </si>
+  <si>
+    <t>137:16:10</t>
+  </si>
+  <si>
+    <t>137:16:22</t>
+  </si>
+  <si>
+    <t>137:16:38</t>
+  </si>
+  <si>
+    <t>137:16:52</t>
+  </si>
+  <si>
+    <t>137:17:04</t>
+  </si>
+  <si>
     <t>138:11:46</t>
-  </si>
-  <si>
-    <t>138:11:50</t>
-  </si>
-  <si>
-    <t>138:12:01</t>
-  </si>
-  <si>
-    <t>138:12:03</t>
-  </si>
-  <si>
-    <t>138:12:06</t>
-  </si>
-  <si>
-    <t>141:29:47</t>
-  </si>
-  <si>
-    <t>141:29:51</t>
-  </si>
-  <si>
-    <t>141:29:53</t>
-  </si>
-  <si>
-    <t>141:29:56</t>
-  </si>
-  <si>
-    <t>141:29:57</t>
-  </si>
-  <si>
-    <t>141:29:59</t>
-  </si>
-  <si>
-    <t>141:30:08</t>
-  </si>
-  <si>
-    <t>141:30:10</t>
-  </si>
-  <si>
-    <t>141:30:12</t>
-  </si>
-  <si>
-    <t>141:30:16</t>
-  </si>
-  <si>
-    <t>141:30:17</t>
-  </si>
-  <si>
-    <t>141:30:18</t>
-  </si>
-  <si>
-    <t>141:30:24</t>
-  </si>
-  <si>
-    <t>141:30:25</t>
-  </si>
-  <si>
-    <t>141:30:26</t>
-  </si>
-  <si>
-    <t>141:30:27</t>
-  </si>
-  <si>
-    <t>009:03:13</t>
-  </si>
-  <si>
-    <t>009:26:36</t>
-  </si>
-  <si>
-    <t>095:50:49</t>
-  </si>
-  <si>
-    <t>095:51:01</t>
-  </si>
-  <si>
-    <t>095:52:38</t>
-  </si>
-  <si>
-    <t>094:15:02</t>
-  </si>
-  <si>
-    <t>094:15:48</t>
-  </si>
-  <si>
-    <t>113:27:01</t>
-  </si>
-  <si>
-    <t>113:27:18</t>
-  </si>
-  <si>
-    <t>113:27:32</t>
-  </si>
-  <si>
-    <t>113:28:37</t>
-  </si>
-  <si>
-    <t>113:28:48</t>
-  </si>
-  <si>
-    <t>113:30:25</t>
-  </si>
-  <si>
-    <t>113:34:48</t>
-  </si>
-  <si>
-    <t>113:35:11</t>
-  </si>
-  <si>
-    <t>113:35:52</t>
-  </si>
-  <si>
-    <t>113:35:59</t>
-  </si>
-  <si>
-    <t>113:36:07</t>
-  </si>
-  <si>
-    <t>113:37:36</t>
-  </si>
-  <si>
-    <t>113:38:21</t>
-  </si>
-  <si>
-    <t>113:38:26</t>
-  </si>
-  <si>
-    <t>113:38:30</t>
-  </si>
-  <si>
-    <t>078:02:20</t>
   </si>
 </sst>
 </file>
@@ -5639,8 +5939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA25AE87-EBB6-4592-B83F-0D7E34AA70ED}">
   <dimension ref="A1:H704"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A607" workbookViewId="0">
-      <selection activeCell="A659" sqref="A659"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7222,7 +7522,7 @@
     </row>
     <row r="98" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="27" t="s">
-        <v>1654</v>
+        <v>1797</v>
       </c>
       <c r="B98" t="s">
         <v>784</v>
@@ -7238,7 +7538,7 @@
     </row>
     <row r="99" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="27" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="B99" t="s">
         <v>786</v>
@@ -7254,7 +7554,7 @@
     </row>
     <row r="100" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="27" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B100" t="s">
         <v>789</v>
@@ -7270,7 +7570,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="27" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B101" t="s">
         <v>790</v>
@@ -7286,7 +7586,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="27" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="B102" t="s">
         <v>791</v>
@@ -7318,7 +7618,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="27" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="B104" t="s">
         <v>799</v>
@@ -7350,7 +7650,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="27" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="B106" t="s">
         <v>801</v>
@@ -7366,7 +7666,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="27" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="B107" t="s">
         <v>802</v>
@@ -7398,7 +7698,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="27" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="B109" t="s">
         <v>804</v>
@@ -7414,7 +7714,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="27" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="B110" t="s">
         <v>805</v>
@@ -7430,7 +7730,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="27" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="B111" t="s">
         <v>806</v>
@@ -7558,7 +7858,7 @@
     </row>
     <row r="119" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="27" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="B119" t="s">
         <v>814</v>
@@ -7574,7 +7874,7 @@
     </row>
     <row r="120" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="27" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="B120" t="s">
         <v>815</v>
@@ -7606,7 +7906,7 @@
     </row>
     <row r="122" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="27" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="B122" t="s">
         <v>817</v>
@@ -7638,7 +7938,7 @@
     </row>
     <row r="124" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="27" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="B124" t="s">
         <v>819</v>
@@ -7654,7 +7954,7 @@
     </row>
     <row r="125" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="27" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="B125" t="s">
         <v>820</v>
@@ -7670,7 +7970,7 @@
     </row>
     <row r="126" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="27" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="B126" t="s">
         <v>821</v>
@@ -7686,7 +7986,7 @@
     </row>
     <row r="127" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="27" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="B127" t="s">
         <v>822</v>
@@ -7702,7 +8002,7 @@
     </row>
     <row r="128" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="27" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="B128" t="s">
         <v>823</v>
@@ -7718,7 +8018,7 @@
     </row>
     <row r="129" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="27" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="B129" t="s">
         <v>824</v>
@@ -7734,7 +8034,7 @@
     </row>
     <row r="130" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="27" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="B130" t="s">
         <v>825</v>
@@ -8006,7 +8306,7 @@
     </row>
     <row r="147" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="27" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="B147" t="s">
         <v>283</v>
@@ -8022,7 +8322,7 @@
     </row>
     <row r="148" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="27" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="B148" t="s">
         <v>284</v>
@@ -9966,7 +10266,7 @@
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="27" t="s">
-        <v>1495</v>
+        <v>1682</v>
       </c>
       <c r="B269" t="s">
         <v>610</v>
@@ -9982,7 +10282,7 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="27" t="s">
-        <v>1496</v>
+        <v>1683</v>
       </c>
       <c r="B270" t="s">
         <v>611</v>
@@ -10030,7 +10330,7 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="27" t="s">
-        <v>70</v>
+        <v>1684</v>
       </c>
       <c r="B273" t="s">
         <v>623</v>
@@ -10046,7 +10346,7 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="27" t="s">
-        <v>71</v>
+        <v>1685</v>
       </c>
       <c r="B274" t="s">
         <v>624</v>
@@ -10110,7 +10410,7 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="27" t="s">
-        <v>1499</v>
+        <v>1686</v>
       </c>
       <c r="B278" t="s">
         <v>659</v>
@@ -10126,7 +10426,7 @@
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="27" t="s">
-        <v>1500</v>
+        <v>1687</v>
       </c>
       <c r="B279" t="s">
         <v>660</v>
@@ -12603,7 +12903,7 @@
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A431" s="27" t="s">
-        <v>252</v>
+        <v>1688</v>
       </c>
       <c r="B431" t="s">
         <v>582</v>
@@ -12619,7 +12919,7 @@
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A432" s="27" t="s">
-        <v>253</v>
+        <v>1689</v>
       </c>
       <c r="B432" t="s">
         <v>584</v>
@@ -12635,7 +12935,7 @@
     </row>
     <row r="433" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A433" s="27" t="s">
-        <v>1346</v>
+        <v>1690</v>
       </c>
       <c r="B433" t="s">
         <v>585</v>
@@ -12651,7 +12951,7 @@
     </row>
     <row r="434" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A434" s="27" t="s">
-        <v>1347</v>
+        <v>1691</v>
       </c>
       <c r="B434" t="s">
         <v>588</v>
@@ -12795,7 +13095,7 @@
     </row>
     <row r="443" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A443" s="27" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="B443" t="s">
         <v>628</v>
@@ -12811,7 +13111,7 @@
     </row>
     <row r="444" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A444" s="27" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="B444" t="s">
         <v>629</v>
@@ -12843,7 +13143,7 @@
     </row>
     <row r="446" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A446" s="27" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="B446" t="s">
         <v>631</v>
@@ -12955,7 +13255,7 @@
     </row>
     <row r="453" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A453" s="27" t="s">
-        <v>82</v>
+        <v>1692</v>
       </c>
       <c r="B453" t="s">
         <v>299</v>
@@ -12971,7 +13271,7 @@
     </row>
     <row r="454" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A454" s="27" t="s">
-        <v>83</v>
+        <v>1693</v>
       </c>
       <c r="B454" t="s">
         <v>300</v>
@@ -12987,7 +13287,7 @@
     </row>
     <row r="455" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A455" s="27" t="s">
-        <v>84</v>
+        <v>1694</v>
       </c>
       <c r="B455" t="s">
         <v>301</v>
@@ -13003,7 +13303,7 @@
     </row>
     <row r="456" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A456" s="27" t="s">
-        <v>1514</v>
+        <v>1695</v>
       </c>
       <c r="B456" t="s">
         <v>302</v>
@@ -13643,7 +13943,7 @@
     </row>
     <row r="496" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A496" s="27" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="B496" t="s">
         <v>621</v>
@@ -13659,7 +13959,7 @@
     </row>
     <row r="497" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A497" s="27" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="B497" t="s">
         <v>622</v>
@@ -13851,7 +14151,7 @@
     </row>
     <row r="509" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A509" s="27" t="s">
-        <v>225</v>
+        <v>1696</v>
       </c>
       <c r="B509" t="s">
         <v>643</v>
@@ -13867,7 +14167,7 @@
     </row>
     <row r="510" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A510" s="27" t="s">
-        <v>203</v>
+        <v>1697</v>
       </c>
       <c r="B510" t="s">
         <v>644</v>
@@ -13883,7 +14183,7 @@
     </row>
     <row r="511" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A511" s="27" t="s">
-        <v>227</v>
+        <v>1698</v>
       </c>
       <c r="B511" t="s">
         <v>645</v>
@@ -13899,7 +14199,7 @@
     </row>
     <row r="512" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A512" s="27" t="s">
-        <v>228</v>
+        <v>1699</v>
       </c>
       <c r="B512" t="s">
         <v>646</v>
@@ -13915,7 +14215,7 @@
     </row>
     <row r="513" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A513" s="27" t="s">
-        <v>229</v>
+        <v>1700</v>
       </c>
       <c r="B513" t="s">
         <v>647</v>
@@ -13931,7 +14231,7 @@
     </row>
     <row r="514" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A514" s="27" t="s">
-        <v>204</v>
+        <v>1701</v>
       </c>
       <c r="B514" t="s">
         <v>648</v>
@@ -13947,7 +14247,7 @@
     </row>
     <row r="515" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A515" s="27" t="s">
-        <v>205</v>
+        <v>1702</v>
       </c>
       <c r="B515" t="s">
         <v>649</v>
@@ -13963,7 +14263,7 @@
     </row>
     <row r="516" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A516" s="27" t="s">
-        <v>206</v>
+        <v>1703</v>
       </c>
       <c r="B516" t="s">
         <v>650</v>
@@ -13979,7 +14279,7 @@
     </row>
     <row r="517" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A517" s="27" t="s">
-        <v>233</v>
+        <v>1704</v>
       </c>
       <c r="B517" t="s">
         <v>651</v>
@@ -13995,7 +14295,7 @@
     </row>
     <row r="518" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A518" s="27" t="s">
-        <v>234</v>
+        <v>1705</v>
       </c>
       <c r="B518" t="s">
         <v>652</v>
@@ -14011,7 +14311,7 @@
     </row>
     <row r="519" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A519" s="27" t="s">
-        <v>235</v>
+        <v>1706</v>
       </c>
       <c r="B519" t="s">
         <v>653</v>
@@ -14027,7 +14327,7 @@
     </row>
     <row r="520" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A520" s="27" t="s">
-        <v>236</v>
+        <v>1707</v>
       </c>
       <c r="B520" t="s">
         <v>654</v>
@@ -14043,7 +14343,7 @@
     </row>
     <row r="521" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A521" s="27" t="s">
-        <v>207</v>
+        <v>1708</v>
       </c>
       <c r="B521" t="s">
         <v>655</v>
@@ -14059,7 +14359,7 @@
     </row>
     <row r="522" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A522" s="27" t="s">
-        <v>238</v>
+        <v>1709</v>
       </c>
       <c r="B522" t="s">
         <v>656</v>
@@ -14075,7 +14375,7 @@
     </row>
     <row r="523" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A523" s="27" t="s">
-        <v>208</v>
+        <v>1710</v>
       </c>
       <c r="B523" t="s">
         <v>657</v>
@@ -14091,7 +14391,7 @@
     </row>
     <row r="524" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A524" s="27" t="s">
-        <v>209</v>
+        <v>1711</v>
       </c>
       <c r="B524" t="s">
         <v>658</v>
@@ -14107,7 +14407,7 @@
     </row>
     <row r="525" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A525" s="27" t="s">
-        <v>1517</v>
+        <v>1712</v>
       </c>
       <c r="B525" t="s">
         <v>661</v>
@@ -14123,7 +14423,7 @@
     </row>
     <row r="526" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A526" s="27" t="s">
-        <v>1518</v>
+        <v>1713</v>
       </c>
       <c r="B526" t="s">
         <v>662</v>
@@ -14139,7 +14439,7 @@
     </row>
     <row r="527" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A527" s="27" t="s">
-        <v>1519</v>
+        <v>1714</v>
       </c>
       <c r="B527" t="s">
         <v>663</v>
@@ -14155,7 +14455,7 @@
     </row>
     <row r="528" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A528" s="27" t="s">
-        <v>1520</v>
+        <v>1715</v>
       </c>
       <c r="B528" t="s">
         <v>664</v>
@@ -14171,7 +14471,7 @@
     </row>
     <row r="529" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A529" s="27" t="s">
-        <v>1572</v>
+        <v>1716</v>
       </c>
       <c r="B529" t="s">
         <v>665</v>
@@ -14187,7 +14487,7 @@
     </row>
     <row r="530" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A530" s="27" t="s">
-        <v>1573</v>
+        <v>1717</v>
       </c>
       <c r="B530" t="s">
         <v>666</v>
@@ -14203,7 +14503,7 @@
     </row>
     <row r="531" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A531" s="27" t="s">
-        <v>1574</v>
+        <v>1718</v>
       </c>
       <c r="B531" t="s">
         <v>667</v>
@@ -14219,7 +14519,7 @@
     </row>
     <row r="532" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A532" s="27" t="s">
-        <v>1209</v>
+        <v>1719</v>
       </c>
       <c r="B532" t="s">
         <v>668</v>
@@ -14235,7 +14535,7 @@
     </row>
     <row r="533" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A533" s="27" t="s">
-        <v>1210</v>
+        <v>1720</v>
       </c>
       <c r="B533" t="s">
         <v>669</v>
@@ -14251,7 +14551,7 @@
     </row>
     <row r="534" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A534" s="27" t="s">
-        <v>1211</v>
+        <v>1721</v>
       </c>
       <c r="B534" t="s">
         <v>670</v>
@@ -14267,7 +14567,7 @@
     </row>
     <row r="535" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A535" s="27" t="s">
-        <v>1575</v>
+        <v>1721</v>
       </c>
       <c r="B535" t="s">
         <v>671</v>
@@ -14283,7 +14583,7 @@
     </row>
     <row r="536" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A536" s="27" t="s">
-        <v>1576</v>
+        <v>1722</v>
       </c>
       <c r="B536" t="s">
         <v>672</v>
@@ -14299,7 +14599,7 @@
     </row>
     <row r="537" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A537" s="27" t="s">
-        <v>1577</v>
+        <v>1723</v>
       </c>
       <c r="B537" t="s">
         <v>673</v>
@@ -14315,7 +14615,7 @@
     </row>
     <row r="538" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A538" s="27" t="s">
-        <v>1578</v>
+        <v>1724</v>
       </c>
       <c r="B538" t="s">
         <v>674</v>
@@ -14331,7 +14631,7 @@
     </row>
     <row r="539" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A539" s="27" t="s">
-        <v>1579</v>
+        <v>1725</v>
       </c>
       <c r="B539" t="s">
         <v>675</v>
@@ -14347,7 +14647,7 @@
     </row>
     <row r="540" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A540" s="27" t="s">
-        <v>1580</v>
+        <v>1726</v>
       </c>
       <c r="B540" t="s">
         <v>676</v>
@@ -14363,7 +14663,7 @@
     </row>
     <row r="541" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A541" s="27" t="s">
-        <v>1581</v>
+        <v>1727</v>
       </c>
       <c r="B541" t="s">
         <v>677</v>
@@ -14379,7 +14679,7 @@
     </row>
     <row r="542" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A542" s="27" t="s">
-        <v>1582</v>
+        <v>1728</v>
       </c>
       <c r="B542" t="s">
         <v>678</v>
@@ -14395,7 +14695,7 @@
     </row>
     <row r="543" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A543" s="27" t="s">
-        <v>1583</v>
+        <v>1729</v>
       </c>
       <c r="B543" t="s">
         <v>679</v>
@@ -14411,7 +14711,7 @@
     </row>
     <row r="544" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A544" s="27" t="s">
-        <v>1584</v>
+        <v>1730</v>
       </c>
       <c r="B544" t="s">
         <v>680</v>
@@ -14443,7 +14743,7 @@
     </row>
     <row r="546" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A546" s="27" t="s">
-        <v>1213</v>
+        <v>1731</v>
       </c>
       <c r="B546" t="s">
         <v>682</v>
@@ -14459,7 +14759,7 @@
     </row>
     <row r="547" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A547" s="27" t="s">
-        <v>1214</v>
+        <v>1732</v>
       </c>
       <c r="B547" t="s">
         <v>683</v>
@@ -14475,7 +14775,7 @@
     </row>
     <row r="548" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A548" s="27" t="s">
-        <v>1215</v>
+        <v>1733</v>
       </c>
       <c r="B548" t="s">
         <v>684</v>
@@ -14491,7 +14791,7 @@
     </row>
     <row r="549" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A549" s="27" t="s">
-        <v>1216</v>
+        <v>1734</v>
       </c>
       <c r="B549" t="s">
         <v>685</v>
@@ -14507,7 +14807,7 @@
     </row>
     <row r="550" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A550" s="27" t="s">
-        <v>1217</v>
+        <v>1735</v>
       </c>
       <c r="B550" t="s">
         <v>686</v>
@@ -14523,7 +14823,7 @@
     </row>
     <row r="551" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A551" s="27" t="s">
-        <v>1218</v>
+        <v>1736</v>
       </c>
       <c r="B551" t="s">
         <v>687</v>
@@ -14539,7 +14839,7 @@
     </row>
     <row r="552" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A552" s="27" t="s">
-        <v>1219</v>
+        <v>1737</v>
       </c>
       <c r="B552" t="s">
         <v>688</v>
@@ -14555,7 +14855,7 @@
     </row>
     <row r="553" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A553" s="27" t="s">
-        <v>1220</v>
+        <v>1738</v>
       </c>
       <c r="B553" t="s">
         <v>689</v>
@@ -14571,7 +14871,7 @@
     </row>
     <row r="554" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A554" s="27" t="s">
-        <v>1221</v>
+        <v>1739</v>
       </c>
       <c r="B554" t="s">
         <v>690</v>
@@ -14587,7 +14887,7 @@
     </row>
     <row r="555" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A555" s="27" t="s">
-        <v>1682</v>
+        <v>1740</v>
       </c>
       <c r="B555" t="s">
         <v>691</v>
@@ -14603,7 +14903,7 @@
     </row>
     <row r="556" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A556" s="27" t="s">
-        <v>1683</v>
+        <v>1741</v>
       </c>
       <c r="B556" t="s">
         <v>692</v>
@@ -14619,7 +14919,7 @@
     </row>
     <row r="557" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A557" s="27" t="s">
-        <v>1684</v>
+        <v>1742</v>
       </c>
       <c r="B557" t="s">
         <v>693</v>
@@ -14635,7 +14935,7 @@
     </row>
     <row r="558" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A558" s="27" t="s">
-        <v>1685</v>
+        <v>1743</v>
       </c>
       <c r="B558" t="s">
         <v>694</v>
@@ -14651,7 +14951,7 @@
     </row>
     <row r="559" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A559" s="27" t="s">
-        <v>1686</v>
+        <v>1744</v>
       </c>
       <c r="B559" t="s">
         <v>695</v>
@@ -14667,7 +14967,7 @@
     </row>
     <row r="560" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A560" s="27" t="s">
-        <v>1687</v>
+        <v>1745</v>
       </c>
       <c r="B560" t="s">
         <v>696</v>
@@ -14683,7 +14983,7 @@
     </row>
     <row r="561" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A561" s="27" t="s">
-        <v>1688</v>
+        <v>1746</v>
       </c>
       <c r="B561" t="s">
         <v>697</v>
@@ -14699,7 +14999,7 @@
     </row>
     <row r="562" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A562" s="27" t="s">
-        <v>1689</v>
+        <v>1747</v>
       </c>
       <c r="B562" t="s">
         <v>698</v>
@@ -14715,7 +15015,7 @@
     </row>
     <row r="563" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A563" s="27" t="s">
-        <v>1690</v>
+        <v>1748</v>
       </c>
       <c r="B563" t="s">
         <v>699</v>
@@ -14731,7 +15031,7 @@
     </row>
     <row r="564" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A564" s="27" t="s">
-        <v>1691</v>
+        <v>1749</v>
       </c>
       <c r="B564" t="s">
         <v>700</v>
@@ -14747,7 +15047,7 @@
     </row>
     <row r="565" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A565" s="27" t="s">
-        <v>1692</v>
+        <v>1750</v>
       </c>
       <c r="B565" t="s">
         <v>701</v>
@@ -14763,7 +15063,7 @@
     </row>
     <row r="566" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A566" s="27" t="s">
-        <v>1693</v>
+        <v>1751</v>
       </c>
       <c r="B566" t="s">
         <v>702</v>
@@ -14779,7 +15079,7 @@
     </row>
     <row r="567" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A567" s="27" t="s">
-        <v>1694</v>
+        <v>1752</v>
       </c>
       <c r="B567" t="s">
         <v>703</v>
@@ -14795,7 +15095,7 @@
     </row>
     <row r="568" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A568" s="27" t="s">
-        <v>1695</v>
+        <v>1753</v>
       </c>
       <c r="B568" t="s">
         <v>704</v>
@@ -14811,7 +15111,7 @@
     </row>
     <row r="569" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A569" s="27" t="s">
-        <v>1696</v>
+        <v>1754</v>
       </c>
       <c r="B569" t="s">
         <v>705</v>
@@ -14827,7 +15127,7 @@
     </row>
     <row r="570" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A570" s="27" t="s">
-        <v>1237</v>
+        <v>1755</v>
       </c>
       <c r="B570" t="s">
         <v>706</v>
@@ -14843,7 +15143,7 @@
     </row>
     <row r="571" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A571" s="27" t="s">
-        <v>1238</v>
+        <v>1756</v>
       </c>
       <c r="B571" t="s">
         <v>707</v>
@@ -14859,7 +15159,7 @@
     </row>
     <row r="572" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A572" s="27" t="s">
-        <v>1239</v>
+        <v>1757</v>
       </c>
       <c r="B572" t="s">
         <v>708</v>
@@ -14875,7 +15175,7 @@
     </row>
     <row r="573" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A573" s="27" t="s">
-        <v>1240</v>
+        <v>1758</v>
       </c>
       <c r="B573" t="s">
         <v>709</v>
@@ -14891,7 +15191,7 @@
     </row>
     <row r="574" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A574" s="27" t="s">
-        <v>1241</v>
+        <v>1759</v>
       </c>
       <c r="B574" t="s">
         <v>710</v>
@@ -14907,7 +15207,7 @@
     </row>
     <row r="575" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A575" s="27" t="s">
-        <v>1242</v>
+        <v>1760</v>
       </c>
       <c r="B575" t="s">
         <v>711</v>
@@ -14923,7 +15223,7 @@
     </row>
     <row r="576" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A576" s="27" t="s">
-        <v>1243</v>
+        <v>1761</v>
       </c>
       <c r="B576" t="s">
         <v>712</v>
@@ -14939,7 +15239,7 @@
     </row>
     <row r="577" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A577" s="27" t="s">
-        <v>1244</v>
+        <v>1762</v>
       </c>
       <c r="B577" t="s">
         <v>713</v>
@@ -14955,7 +15255,7 @@
     </row>
     <row r="578" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A578" s="27" t="s">
-        <v>1245</v>
+        <v>1763</v>
       </c>
       <c r="B578" t="s">
         <v>714</v>
@@ -14971,7 +15271,7 @@
     </row>
     <row r="579" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A579" s="27" t="s">
-        <v>1246</v>
+        <v>1764</v>
       </c>
       <c r="B579" t="s">
         <v>715</v>
@@ -14987,7 +15287,7 @@
     </row>
     <row r="580" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A580" s="27" t="s">
-        <v>1247</v>
+        <v>1765</v>
       </c>
       <c r="B580" t="s">
         <v>716</v>
@@ -15003,7 +15303,7 @@
     </row>
     <row r="581" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A581" s="27" t="s">
-        <v>1248</v>
+        <v>1764</v>
       </c>
       <c r="B581" t="s">
         <v>717</v>
@@ -15020,7 +15320,7 @@
     </row>
     <row r="582" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A582" s="27" t="s">
-        <v>1249</v>
+        <v>1766</v>
       </c>
       <c r="B582" t="s">
         <v>718</v>
@@ -15036,7 +15336,7 @@
     </row>
     <row r="583" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A583" s="27" t="s">
-        <v>1250</v>
+        <v>1767</v>
       </c>
       <c r="B583" t="s">
         <v>719</v>
@@ -15052,7 +15352,7 @@
     </row>
     <row r="584" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A584" s="27" t="s">
-        <v>1251</v>
+        <v>1768</v>
       </c>
       <c r="B584" t="s">
         <v>720</v>
@@ -15068,7 +15368,7 @@
     </row>
     <row r="585" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A585" s="27" t="s">
-        <v>1252</v>
+        <v>1769</v>
       </c>
       <c r="B585" t="s">
         <v>721</v>
@@ -15084,7 +15384,7 @@
     </row>
     <row r="586" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A586" s="27" t="s">
-        <v>1253</v>
+        <v>1770</v>
       </c>
       <c r="B586" t="s">
         <v>722</v>
@@ -15100,7 +15400,7 @@
     </row>
     <row r="587" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A587" s="27" t="s">
-        <v>1254</v>
+        <v>1771</v>
       </c>
       <c r="B587" t="s">
         <v>723</v>
@@ -15116,7 +15416,7 @@
     </row>
     <row r="588" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A588" s="27" t="s">
-        <v>1255</v>
+        <v>1772</v>
       </c>
       <c r="B588" t="s">
         <v>724</v>
@@ -15132,7 +15432,7 @@
     </row>
     <row r="589" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A589" s="27" t="s">
-        <v>1256</v>
+        <v>1773</v>
       </c>
       <c r="B589" t="s">
         <v>725</v>
@@ -15148,7 +15448,7 @@
     </row>
     <row r="590" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A590" s="27" t="s">
-        <v>1257</v>
+        <v>1774</v>
       </c>
       <c r="B590" t="s">
         <v>726</v>
@@ -15164,7 +15464,7 @@
     </row>
     <row r="591" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A591" s="27" t="s">
-        <v>1258</v>
+        <v>1775</v>
       </c>
       <c r="B591" t="s">
         <v>727</v>
@@ -15180,7 +15480,7 @@
     </row>
     <row r="592" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A592" s="27" t="s">
-        <v>1259</v>
+        <v>1776</v>
       </c>
       <c r="B592" t="s">
         <v>728</v>
@@ -15196,7 +15496,7 @@
     </row>
     <row r="593" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A593" s="27" t="s">
-        <v>1260</v>
+        <v>1777</v>
       </c>
       <c r="B593" t="s">
         <v>729</v>
@@ -15212,7 +15512,7 @@
     </row>
     <row r="594" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A594" s="27" t="s">
-        <v>1261</v>
+        <v>1778</v>
       </c>
       <c r="B594" t="s">
         <v>730</v>
@@ -15228,7 +15528,7 @@
     </row>
     <row r="595" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A595" s="27" t="s">
-        <v>1262</v>
+        <v>1779</v>
       </c>
       <c r="B595" t="s">
         <v>731</v>
@@ -15244,7 +15544,7 @@
     </row>
     <row r="596" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A596" s="27" t="s">
-        <v>1263</v>
+        <v>1780</v>
       </c>
       <c r="B596" t="s">
         <v>732</v>
@@ -15260,7 +15560,7 @@
     </row>
     <row r="597" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A597" s="27" t="s">
-        <v>1264</v>
+        <v>1781</v>
       </c>
       <c r="B597" t="s">
         <v>733</v>
@@ -15276,7 +15576,7 @@
     </row>
     <row r="598" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A598" s="27" t="s">
-        <v>1265</v>
+        <v>1782</v>
       </c>
       <c r="B598" t="s">
         <v>734</v>
@@ -15292,7 +15592,7 @@
     </row>
     <row r="599" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A599" s="27" t="s">
-        <v>1266</v>
+        <v>1783</v>
       </c>
       <c r="B599" t="s">
         <v>735</v>
@@ -15308,7 +15608,7 @@
     </row>
     <row r="600" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A600" s="27" t="s">
-        <v>1267</v>
+        <v>1784</v>
       </c>
       <c r="B600" t="s">
         <v>736</v>
@@ -15324,7 +15624,7 @@
     </row>
     <row r="601" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A601" s="27" t="s">
-        <v>1268</v>
+        <v>1785</v>
       </c>
       <c r="B601" t="s">
         <v>737</v>
@@ -15340,7 +15640,7 @@
     </row>
     <row r="602" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A602" s="27" t="s">
-        <v>1269</v>
+        <v>1786</v>
       </c>
       <c r="B602" t="s">
         <v>738</v>
@@ -15356,7 +15656,7 @@
     </row>
     <row r="603" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A603" s="27" t="s">
-        <v>1270</v>
+        <v>1787</v>
       </c>
       <c r="B603" t="s">
         <v>739</v>
@@ -15372,7 +15672,7 @@
     </row>
     <row r="604" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A604" s="27" t="s">
-        <v>1271</v>
+        <v>1788</v>
       </c>
       <c r="B604" t="s">
         <v>740</v>
@@ -15388,7 +15688,7 @@
     </row>
     <row r="605" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A605" s="27" t="s">
-        <v>1585</v>
+        <v>1789</v>
       </c>
       <c r="B605" t="s">
         <v>741</v>
@@ -15404,7 +15704,7 @@
     </row>
     <row r="606" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A606" s="27" t="s">
-        <v>1586</v>
+        <v>1790</v>
       </c>
       <c r="B606" t="s">
         <v>742</v>
@@ -15436,7 +15736,7 @@
     </row>
     <row r="608" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A608" s="27" t="s">
-        <v>1272</v>
+        <v>1791</v>
       </c>
       <c r="B608" t="s">
         <v>792</v>
@@ -15452,7 +15752,7 @@
     </row>
     <row r="609" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A609" s="27" t="s">
-        <v>1273</v>
+        <v>1792</v>
       </c>
       <c r="B609" t="s">
         <v>793</v>
@@ -15468,7 +15768,7 @@
     </row>
     <row r="610" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A610" s="27" t="s">
-        <v>1274</v>
+        <v>1793</v>
       </c>
       <c r="B610" t="s">
         <v>794</v>
@@ -15484,7 +15784,7 @@
     </row>
     <row r="611" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A611" s="27" t="s">
-        <v>1275</v>
+        <v>1794</v>
       </c>
       <c r="B611" t="s">
         <v>795</v>
@@ -15500,7 +15800,7 @@
     </row>
     <row r="612" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A612" s="27" t="s">
-        <v>1276</v>
+        <v>1795</v>
       </c>
       <c r="B612" t="s">
         <v>796</v>
@@ -15516,7 +15816,7 @@
     </row>
     <row r="613" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A613" s="27" t="s">
-        <v>1277</v>
+        <v>1796</v>
       </c>
       <c r="B613" t="s">
         <v>797</v>
@@ -16298,7 +16598,7 @@
     </row>
     <row r="657" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A657" s="24" t="s">
-        <v>1697</v>
+        <v>1681</v>
       </c>
       <c r="B657" s="3" t="s">
         <v>1588</v>

</xml_diff>

<commit_message>
photo corrections from Robin debugging graph overlay
</commit_message>
<xml_diff>
--- a/MISSION_DATA/A13_photos.xlsx
+++ b/MISSION_DATA/A13_photos.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apollo_13\MISSION_DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Spaceflight\Apollo\Apollo 13\Apollo 13 Handheld photography\Apollo 13 GET Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A331F70-DE2C-4843-B328-B7878380191A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC0E930-2F9B-4A14-A5DD-CC6C4374306F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="4260" windowWidth="38535" windowHeight="23985" xr2:uid="{E7285D04-3DFB-428F-BD58-901528569A82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E7285D04-3DFB-428F-BD58-901528569A82}"/>
   </bookViews>
   <sheets>
     <sheet name="A13_photos" sheetId="15" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="16" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4660" uniqueCount="1798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4660" uniqueCount="1804">
   <si>
     <t>LM &amp; S-IVB during Transposition and Docking</t>
   </si>
@@ -5462,6 +5462,24 @@
   </si>
   <si>
     <t>138:11:46</t>
+  </si>
+  <si>
+    <t>Edge of Command Module with small Lunar Disc and SM on extreme left of frame, taken by CDR through the LM docking window as pitch up continues</t>
+  </si>
+  <si>
+    <t>Swigert &amp; Lovell working on air lines in LM. Double LioH canister by ECS</t>
+  </si>
+  <si>
+    <t>Lunar disc looking east with Mare Smythii and Mare Undarum through the LM AOT. The CSM EVA floodlight is visible</t>
+  </si>
+  <si>
+    <t>Apollo 13 Saturn V spot lit on the launch pad</t>
+  </si>
+  <si>
+    <t>Earth, western Africa</t>
+  </si>
+  <si>
+    <t>Earth, eastern Atlantic Ocean</t>
   </si>
 </sst>
 </file>
@@ -5939,8 +5957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA25AE87-EBB6-4592-B83F-0D7E34AA70ED}">
   <dimension ref="A1:H704"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E601" sqref="E601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6954,7 +6972,7 @@
       <c r="C62" s="22"/>
       <c r="D62" s="15"/>
       <c r="E62" s="17" t="s">
-        <v>1158</v>
+        <v>1798</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>1591</v>
@@ -6970,7 +6988,7 @@
       <c r="C63" s="22"/>
       <c r="D63" s="15"/>
       <c r="E63" s="17" t="s">
-        <v>1158</v>
+        <v>1798</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>1591</v>
@@ -6986,7 +7004,7 @@
       <c r="C64" s="22"/>
       <c r="D64" s="15"/>
       <c r="E64" s="17" t="s">
-        <v>1158</v>
+        <v>1798</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>1591</v>
@@ -7002,7 +7020,7 @@
       <c r="C65" s="22"/>
       <c r="D65" s="15"/>
       <c r="E65" s="17" t="s">
-        <v>1158</v>
+        <v>1798</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>1591</v>
@@ -7018,7 +7036,7 @@
       <c r="C66" s="22"/>
       <c r="D66" s="15"/>
       <c r="E66" s="17" t="s">
-        <v>1158</v>
+        <v>1798</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>1591</v>
@@ -7034,7 +7052,7 @@
       <c r="C67" s="22"/>
       <c r="D67" s="15"/>
       <c r="E67" s="17" t="s">
-        <v>1158</v>
+        <v>1798</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>1591</v>
@@ -7050,7 +7068,7 @@
       <c r="C68" s="22"/>
       <c r="D68" s="15"/>
       <c r="E68" s="17" t="s">
-        <v>1158</v>
+        <v>1798</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>1591</v>
@@ -7066,7 +7084,7 @@
       <c r="C69" s="22"/>
       <c r="D69" s="15"/>
       <c r="E69" s="17" t="s">
-        <v>1158</v>
+        <v>1798</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>1591</v>
@@ -7082,7 +7100,7 @@
       <c r="C70" s="22"/>
       <c r="D70" s="15"/>
       <c r="E70" s="17" t="s">
-        <v>1158</v>
+        <v>1798</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>1591</v>
@@ -10674,7 +10692,7 @@
       <c r="C294" s="14"/>
       <c r="D294" s="15"/>
       <c r="E294" s="17" t="s">
-        <v>102</v>
+        <v>1800</v>
       </c>
       <c r="F294" s="1" t="s">
         <v>1591</v>
@@ -10690,7 +10708,7 @@
       <c r="C295" s="14"/>
       <c r="D295" s="15"/>
       <c r="E295" s="17" t="s">
-        <v>102</v>
+        <v>1800</v>
       </c>
       <c r="F295" s="1" t="s">
         <v>1591</v>
@@ -10706,7 +10724,7 @@
       <c r="C296" s="14"/>
       <c r="D296" s="15"/>
       <c r="E296" s="17" t="s">
-        <v>102</v>
+        <v>1800</v>
       </c>
       <c r="F296" s="1" t="s">
         <v>1591</v>
@@ -10722,7 +10740,7 @@
       <c r="C297" s="14"/>
       <c r="D297" s="15"/>
       <c r="E297" s="17" t="s">
-        <v>102</v>
+        <v>1800</v>
       </c>
       <c r="F297" s="1" t="s">
         <v>1591</v>
@@ -10738,7 +10756,7 @@
       <c r="C298" s="14"/>
       <c r="D298" s="15"/>
       <c r="E298" s="17" t="s">
-        <v>102</v>
+        <v>1800</v>
       </c>
       <c r="F298" s="1" t="s">
         <v>1591</v>
@@ -11428,7 +11446,7 @@
       <c r="C341" s="14"/>
       <c r="D341" s="15"/>
       <c r="E341" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F341" s="1" t="s">
         <v>1591</v>
@@ -11445,7 +11463,7 @@
       <c r="C342" s="14"/>
       <c r="D342" s="15"/>
       <c r="E342" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F342" s="1" t="s">
         <v>1591</v>
@@ -11461,7 +11479,7 @@
       <c r="C343" s="14"/>
       <c r="D343" s="15"/>
       <c r="E343" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F343" s="1" t="s">
         <v>1591</v>
@@ -11478,7 +11496,7 @@
       <c r="C344" s="14"/>
       <c r="D344" s="15"/>
       <c r="E344" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F344" s="1" t="s">
         <v>1591</v>
@@ -11494,7 +11512,7 @@
       <c r="C345" s="14"/>
       <c r="D345" s="15"/>
       <c r="E345" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F345" s="1" t="s">
         <v>1591</v>
@@ -11510,7 +11528,7 @@
       <c r="C346" s="14"/>
       <c r="D346" s="15"/>
       <c r="E346" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F346" s="1" t="s">
         <v>1591</v>
@@ -11527,7 +11545,7 @@
       <c r="C347" s="14"/>
       <c r="D347" s="15"/>
       <c r="E347" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F347" s="1" t="s">
         <v>1591</v>
@@ -11543,7 +11561,7 @@
       <c r="C348" s="14"/>
       <c r="D348" s="15"/>
       <c r="E348" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F348" s="1" t="s">
         <v>1591</v>
@@ -11559,7 +11577,7 @@
       <c r="C349" s="14"/>
       <c r="D349" s="15"/>
       <c r="E349" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F349" s="1" t="s">
         <v>1591</v>
@@ -11575,7 +11593,7 @@
       <c r="C350" s="14"/>
       <c r="D350" s="15"/>
       <c r="E350" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F350" s="1" t="s">
         <v>1591</v>
@@ -11592,7 +11610,7 @@
       <c r="C351" s="14"/>
       <c r="D351" s="15"/>
       <c r="E351" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F351" s="1" t="s">
         <v>1591</v>
@@ -11608,7 +11626,7 @@
       <c r="C352" s="14"/>
       <c r="D352" s="15"/>
       <c r="E352" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F352" s="1" t="s">
         <v>1591</v>
@@ -11625,7 +11643,7 @@
       <c r="C353" s="14"/>
       <c r="D353" s="15"/>
       <c r="E353" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F353" s="1" t="s">
         <v>1591</v>
@@ -11642,7 +11660,7 @@
       <c r="C354" s="14"/>
       <c r="D354" s="15"/>
       <c r="E354" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F354" s="1" t="s">
         <v>1591</v>
@@ -11659,7 +11677,7 @@
       <c r="C355" s="14"/>
       <c r="D355" s="15"/>
       <c r="E355" s="20" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="F355" s="1" t="s">
         <v>1591</v>
@@ -15135,7 +15153,7 @@
       <c r="C570" s="14"/>
       <c r="D570" s="15"/>
       <c r="E570" s="17" t="s">
-        <v>241</v>
+        <v>1799</v>
       </c>
       <c r="F570" s="1" t="s">
         <v>1591</v>
@@ -15151,7 +15169,7 @@
       <c r="C571" s="14"/>
       <c r="D571" s="15"/>
       <c r="E571" s="17" t="s">
-        <v>241</v>
+        <v>1799</v>
       </c>
       <c r="F571" s="1" t="s">
         <v>1591</v>
@@ -15167,7 +15185,7 @@
       <c r="C572" s="14"/>
       <c r="D572" s="15"/>
       <c r="E572" s="17" t="s">
-        <v>241</v>
+        <v>1799</v>
       </c>
       <c r="F572" s="1" t="s">
         <v>1591</v>
@@ -15376,7 +15394,7 @@
       <c r="C585" s="14"/>
       <c r="D585" s="15"/>
       <c r="E585" s="17" t="s">
-        <v>195</v>
+        <v>1802</v>
       </c>
       <c r="F585" s="1" t="s">
         <v>1591</v>
@@ -15392,7 +15410,7 @@
       <c r="C586" s="14"/>
       <c r="D586" s="15"/>
       <c r="E586" s="17" t="s">
-        <v>195</v>
+        <v>1802</v>
       </c>
       <c r="F586" s="1" t="s">
         <v>1591</v>
@@ -15408,7 +15426,7 @@
       <c r="C587" s="14"/>
       <c r="D587" s="15"/>
       <c r="E587" s="17" t="s">
-        <v>195</v>
+        <v>1802</v>
       </c>
       <c r="F587" s="1" t="s">
         <v>1591</v>
@@ -15472,7 +15490,7 @@
       <c r="C591" s="14"/>
       <c r="D591" s="15"/>
       <c r="E591" s="17" t="s">
-        <v>196</v>
+        <v>1803</v>
       </c>
       <c r="F591" s="1" t="s">
         <v>1591</v>
@@ -15488,7 +15506,7 @@
       <c r="C592" s="14"/>
       <c r="D592" s="15"/>
       <c r="E592" s="17" t="s">
-        <v>196</v>
+        <v>1803</v>
       </c>
       <c r="F592" s="1" t="s">
         <v>1591</v>
@@ -15504,7 +15522,7 @@
       <c r="C593" s="14"/>
       <c r="D593" s="15"/>
       <c r="E593" s="17" t="s">
-        <v>196</v>
+        <v>1803</v>
       </c>
       <c r="F593" s="1" t="s">
         <v>1591</v>
@@ -15520,7 +15538,7 @@
       <c r="C594" s="14"/>
       <c r="D594" s="15"/>
       <c r="E594" s="17" t="s">
-        <v>196</v>
+        <v>1803</v>
       </c>
       <c r="F594" s="1" t="s">
         <v>1591</v>
@@ -15536,7 +15554,7 @@
       <c r="C595" s="14"/>
       <c r="D595" s="15"/>
       <c r="E595" s="17" t="s">
-        <v>196</v>
+        <v>1803</v>
       </c>
       <c r="F595" s="1" t="s">
         <v>1591</v>
@@ -16016,7 +16034,7 @@
       </c>
       <c r="D624" s="11"/>
       <c r="E624" s="11" t="s">
-        <v>881</v>
+        <v>1801</v>
       </c>
       <c r="F624" s="1" t="s">
         <v>1591</v>
@@ -16755,7 +16773,7 @@
       <c r="A704" s="24"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E658">
+  <sortState ref="A2:E658">
     <sortCondition ref="B2:B658"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>